<commit_message>
manual fix for Program 1 conversion to binary
also add the branch prediction and speculative execution design diagram
</commit_message>
<xml_diff>
--- a/Convert to Binary_v3 - Program 1.xlsx
+++ b/Convert to Binary_v3 - Program 1.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="321">
   <si>
     <t>LDX 1,0,29</t>
   </si>
@@ -983,6 +983,15 @@
   </si>
   <si>
     <t>10111</t>
+  </si>
+  <si>
+    <t>00001010</t>
+  </si>
+  <si>
+    <t>00010101</t>
+  </si>
+  <si>
+    <t>00011111</t>
   </si>
 </sst>
 </file>
@@ -2572,10 +2581,10 @@
   <dimension ref="A1:AD248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M125" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="R7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z149" sqref="Z149"/>
+      <selection pane="bottomRight" activeCell="Y18" sqref="Y18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4645,9 +4654,8 @@
         <f t="shared" si="25"/>
         <v>11</v>
       </c>
-      <c r="Y18" s="10" t="str">
-        <f t="shared" si="26"/>
-        <v>00000000</v>
+      <c r="Y18" s="15" t="s">
+        <v>320</v>
       </c>
       <c r="Z18" s="10" t="str">
         <f t="shared" si="27"/>
@@ -4659,7 +4667,7 @@
       </c>
       <c r="AB18" s="11" t="str">
         <f t="shared" si="29"/>
-        <v>0001101100000000</v>
+        <v>0001101100011111</v>
       </c>
       <c r="AC18" s="10">
         <f t="shared" si="30"/>
@@ -4877,9 +4885,8 @@
         <f t="shared" si="25"/>
         <v>11</v>
       </c>
-      <c r="Y20" s="10" t="str">
-        <f t="shared" si="26"/>
-        <v>00000000</v>
+      <c r="Y20" s="15" t="s">
+        <v>320</v>
       </c>
       <c r="Z20" s="10" t="str">
         <f t="shared" si="27"/>
@@ -4891,7 +4898,7 @@
       </c>
       <c r="AB20" s="11" t="str">
         <f t="shared" si="29"/>
-        <v>0001101100000000</v>
+        <v>0001101100011111</v>
       </c>
       <c r="AC20" s="10">
         <f t="shared" si="30"/>
@@ -5576,9 +5583,8 @@
         <f t="shared" si="25"/>
         <v>11</v>
       </c>
-      <c r="Y26" s="10" t="str">
-        <f t="shared" si="26"/>
-        <v>00000000</v>
+      <c r="Y26" s="15" t="s">
+        <v>318</v>
       </c>
       <c r="Z26" s="10" t="str">
         <f t="shared" si="27"/>
@@ -5590,7 +5596,7 @@
       </c>
       <c r="AB26" s="11" t="str">
         <f t="shared" si="29"/>
-        <v>0001101100000000</v>
+        <v>0001101100001010</v>
       </c>
       <c r="AC26" s="10">
         <f t="shared" si="30"/>
@@ -5808,9 +5814,8 @@
         <f t="shared" si="25"/>
         <v>11</v>
       </c>
-      <c r="Y28" s="10" t="str">
-        <f t="shared" si="26"/>
-        <v>00000000</v>
+      <c r="Y28" s="15" t="s">
+        <v>319</v>
       </c>
       <c r="Z28" s="10" t="str">
         <f t="shared" si="27"/>
@@ -5822,7 +5827,7 @@
       </c>
       <c r="AB28" s="11" t="str">
         <f t="shared" si="29"/>
-        <v>0001101100000000</v>
+        <v>0001101100010101</v>
       </c>
       <c r="AC28" s="10">
         <f t="shared" si="30"/>

</xml_diff>

<commit_message>
programmatic fix for Program 1 conversion to binary
</commit_message>
<xml_diff>
--- a/Convert to Binary_v3 - Program 1.xlsx
+++ b/Convert to Binary_v3 - Program 1.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="313">
   <si>
     <t>LDX 1,0,29</t>
   </si>
@@ -946,18 +946,6 @@
     <t>LDA 3,0,0,binary 10101</t>
   </si>
   <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>11111</t>
-  </si>
-  <si>
-    <t>10101</t>
-  </si>
-  <si>
-    <t>01010</t>
-  </si>
-  <si>
     <t>AIR 3,30</t>
   </si>
   <si>
@@ -980,18 +968,6 @@
   </si>
   <si>
     <t>AIR 3,10</t>
-  </si>
-  <si>
-    <t>10111</t>
-  </si>
-  <si>
-    <t>00001010</t>
-  </si>
-  <si>
-    <t>00010101</t>
-  </si>
-  <si>
-    <t>00011111</t>
   </si>
 </sst>
 </file>
@@ -1165,7 +1141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1207,6 +1183,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1548,12 +1525,12 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1571,7 +1548,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F11" t="s">
         <v>148</v>
@@ -1579,7 +1556,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1613,7 +1590,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D17" t="s">
         <v>153</v>
@@ -1626,7 +1603,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D19" t="s">
         <v>154</v>
@@ -1639,7 +1616,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F21" t="s">
         <v>156</v>
@@ -1671,7 +1648,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1681,7 +1658,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1710,7 +1687,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -2038,7 +2015,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -2192,7 +2169,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F95" t="s">
         <v>254</v>
@@ -2200,7 +2177,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -2581,10 +2558,10 @@
   <dimension ref="A1:AD248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y18" sqref="Y18"/>
+      <selection pane="bottomRight" activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2766,16 +2743,17 @@
         <f t="shared" ref="S2:U2" si="3">DEC2BIN(I2)</f>
         <v>11</v>
       </c>
-      <c r="T2" s="17" t="str">
-        <f t="shared" si="3"/>
+      <c r="T2" s="25" t="str">
+        <f>IF(ISNUMBER(SEARCH("binary", J2)),MID(J2, 8, 5),DEC2BIN(J2))</f>
         <v>0</v>
       </c>
       <c r="U2" s="17" t="str">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="V2" s="17" t="s">
-        <v>305</v>
+      <c r="V2" s="25" t="str">
+        <f>IF(ISNUMBER(SEARCH("binary", L2)),MID(L2, 8, 5),DEC2BIN(L2))</f>
+        <v>101</v>
       </c>
       <c r="W2" s="15" t="str">
         <f t="shared" ref="W2" si="4">R2</f>
@@ -2882,16 +2860,16 @@
         <f t="shared" ref="S3:S66" si="20">DEC2BIN(I3)</f>
         <v>11</v>
       </c>
-      <c r="T3" s="17" t="str">
-        <f t="shared" ref="T3:T66" si="21">DEC2BIN(J3)</f>
+      <c r="T3" s="25" t="str">
+        <f t="shared" ref="T3:T66" si="21">IF(ISNUMBER(SEARCH("binary", J3)),MID(J3, 8, 5),DEC2BIN(J3))</f>
         <v>1</v>
       </c>
       <c r="U3" s="17" t="str">
         <f t="shared" ref="U3:U66" si="22">DEC2BIN(K3)</f>
         <v>1</v>
       </c>
-      <c r="V3" s="17" t="str">
-        <f t="shared" ref="V3:V66" si="23">DEC2BIN(L3)</f>
+      <c r="V3" s="25" t="str">
+        <f t="shared" ref="V3:V66" si="23">IF(ISNUMBER(SEARCH("binary", L3)),MID(L3, 8, 5),DEC2BIN(L3))</f>
         <v>101</v>
       </c>
       <c r="W3" s="15" t="str">
@@ -2999,7 +2977,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T4" s="17" t="str">
+      <c r="T4" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -3007,7 +2985,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V4" s="17" t="str">
+      <c r="V4" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -3116,7 +3094,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T5" s="17" t="str">
+      <c r="T5" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -3124,7 +3102,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V5" s="17" t="str">
+      <c r="V5" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11101</v>
       </c>
@@ -3233,7 +3211,7 @@
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="T6" s="17" t="str">
+      <c r="T6" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -3241,7 +3219,7 @@
         <f t="shared" si="22"/>
         <v>11101</v>
       </c>
-      <c r="V6" s="17" t="str">
+      <c r="V6" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -3350,7 +3328,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T7" s="17" t="str">
+      <c r="T7" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -3358,7 +3336,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V7" s="17" t="str">
+      <c r="V7" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11110</v>
       </c>
@@ -3393,7 +3371,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B8" s="9" t="str">
         <f t="shared" si="8"/>
@@ -3467,7 +3445,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T8" s="17" t="str">
+      <c r="T8" s="25" t="str">
         <f t="shared" si="21"/>
         <v>11110</v>
       </c>
@@ -3475,7 +3453,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V8" s="17" t="str">
+      <c r="V8" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -3510,7 +3488,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B9" s="9" t="str">
         <f t="shared" si="8"/>
@@ -3584,7 +3562,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T9" s="17" t="str">
+      <c r="T9" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1001</v>
       </c>
@@ -3592,7 +3570,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V9" s="17" t="str">
+      <c r="V9" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -3701,7 +3679,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T10" s="17" t="str">
+      <c r="T10" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -3709,7 +3687,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V10" s="17" t="str">
+      <c r="V10" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11101</v>
       </c>
@@ -3818,7 +3796,7 @@
         <f t="shared" si="20"/>
         <v>10</v>
       </c>
-      <c r="T11" s="17" t="str">
+      <c r="T11" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -3826,7 +3804,7 @@
         <f t="shared" si="22"/>
         <v>11101</v>
       </c>
-      <c r="V11" s="17" t="str">
+      <c r="V11" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -3861,7 +3839,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B12" s="9" t="str">
         <f t="shared" si="8"/>
@@ -3935,7 +3913,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T12" s="17" t="str">
+      <c r="T12" s="25" t="str">
         <f t="shared" si="21"/>
         <v>11110</v>
       </c>
@@ -3943,7 +3921,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V12" s="17" t="str">
+      <c r="V12" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -3978,7 +3956,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B13" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4052,7 +4030,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T13" s="17" t="str">
+      <c r="T13" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1001</v>
       </c>
@@ -4060,7 +4038,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V13" s="17" t="str">
+      <c r="V13" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -4169,7 +4147,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T14" s="17" t="str">
+      <c r="T14" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -4177,7 +4155,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V14" s="17" t="str">
+      <c r="V14" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11101</v>
       </c>
@@ -4286,7 +4264,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T15" s="17" t="str">
+      <c r="T15" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -4294,7 +4272,7 @@
         <f t="shared" si="22"/>
         <v>11101</v>
       </c>
-      <c r="V15" s="17" t="str">
+      <c r="V15" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -4403,7 +4381,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T16" s="17" t="str">
+      <c r="T16" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -4411,8 +4389,9 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V16" s="17" t="s">
-        <v>306</v>
+      <c r="V16" s="25" t="str">
+        <f t="shared" si="23"/>
+        <v>11111</v>
       </c>
       <c r="W16" s="15" t="str">
         <f t="shared" si="24"/>
@@ -4519,7 +4498,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T17" s="17" t="str">
+      <c r="T17" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -4527,7 +4506,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="V17" s="17" t="str">
+      <c r="V17" s="25" t="str">
         <f t="shared" si="23"/>
         <v>101</v>
       </c>
@@ -4562,7 +4541,7 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B18" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4636,15 +4615,17 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T18" s="17" t="s">
-        <v>102</v>
+      <c r="T18" s="25" t="str">
+        <f t="shared" si="21"/>
+        <v>11111</v>
       </c>
       <c r="U18" s="17" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V18" s="17" t="s">
-        <v>306</v>
+      <c r="V18" s="25" t="str">
+        <f t="shared" si="23"/>
+        <v>0</v>
       </c>
       <c r="W18" s="15" t="str">
         <f t="shared" si="24"/>
@@ -4654,8 +4635,9 @@
         <f t="shared" si="25"/>
         <v>11</v>
       </c>
-      <c r="Y18" s="15" t="s">
-        <v>320</v>
+      <c r="Y18" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v>00011111</v>
       </c>
       <c r="Z18" s="10" t="str">
         <f t="shared" si="27"/>
@@ -4750,7 +4732,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T19" s="17" t="str">
+      <c r="T19" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -4758,7 +4740,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="V19" s="17" t="str">
+      <c r="V19" s="25" t="str">
         <f t="shared" si="23"/>
         <v>101</v>
       </c>
@@ -4793,7 +4775,7 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B20" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4867,15 +4849,17 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T20" s="17" t="s">
-        <v>102</v>
+      <c r="T20" s="25" t="str">
+        <f t="shared" si="21"/>
+        <v>11111</v>
       </c>
       <c r="U20" s="17" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V20" s="17" t="s">
-        <v>306</v>
+      <c r="V20" s="25" t="str">
+        <f t="shared" si="23"/>
+        <v>0</v>
       </c>
       <c r="W20" s="15" t="str">
         <f t="shared" si="24"/>
@@ -4885,8 +4869,9 @@
         <f t="shared" si="25"/>
         <v>11</v>
       </c>
-      <c r="Y20" s="15" t="s">
-        <v>320</v>
+      <c r="Y20" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v>00011111</v>
       </c>
       <c r="Z20" s="10" t="str">
         <f t="shared" si="27"/>
@@ -4981,7 +4966,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T21" s="17" t="str">
+      <c r="T21" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -4989,7 +4974,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="V21" s="17" t="str">
+      <c r="V21" s="25" t="str">
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
@@ -5024,7 +5009,7 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B22" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5098,7 +5083,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T22" s="17" t="str">
+      <c r="T22" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -5106,7 +5091,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V22" s="17" t="str">
+      <c r="V22" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -5215,7 +5200,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T23" s="17" t="str">
+      <c r="T23" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -5223,7 +5208,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V23" s="17" t="str">
+      <c r="V23" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11000</v>
       </c>
@@ -5332,7 +5317,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T24" s="17" t="str">
+      <c r="T24" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -5340,8 +5325,9 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V24" s="17" t="s">
-        <v>307</v>
+      <c r="V24" s="25" t="str">
+        <f t="shared" si="23"/>
+        <v>10101</v>
       </c>
       <c r="W24" s="15" t="str">
         <f t="shared" si="24"/>
@@ -5448,7 +5434,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T25" s="17" t="str">
+      <c r="T25" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -5456,7 +5442,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="V25" s="17" t="str">
+      <c r="V25" s="25" t="str">
         <f t="shared" si="23"/>
         <v>101</v>
       </c>
@@ -5491,7 +5477,7 @@
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B26" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5565,15 +5551,17 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T26" s="17" t="s">
-        <v>102</v>
+      <c r="T26" s="25" t="str">
+        <f t="shared" si="21"/>
+        <v>01010</v>
       </c>
       <c r="U26" s="17" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V26" s="17" t="s">
-        <v>308</v>
+      <c r="V26" s="25" t="str">
+        <f t="shared" si="23"/>
+        <v>0</v>
       </c>
       <c r="W26" s="15" t="str">
         <f t="shared" si="24"/>
@@ -5583,8 +5571,9 @@
         <f t="shared" si="25"/>
         <v>11</v>
       </c>
-      <c r="Y26" s="15" t="s">
-        <v>318</v>
+      <c r="Y26" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v>00001010</v>
       </c>
       <c r="Z26" s="10" t="str">
         <f t="shared" si="27"/>
@@ -5679,7 +5668,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T27" s="17" t="str">
+      <c r="T27" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -5687,7 +5676,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="V27" s="17" t="str">
+      <c r="V27" s="25" t="str">
         <f t="shared" si="23"/>
         <v>101</v>
       </c>
@@ -5722,7 +5711,7 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B28" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5796,15 +5785,17 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T28" s="17" t="s">
-        <v>102</v>
+      <c r="T28" s="25" t="str">
+        <f t="shared" si="21"/>
+        <v>10101</v>
       </c>
       <c r="U28" s="17" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V28" s="17" t="s">
-        <v>307</v>
+      <c r="V28" s="25" t="str">
+        <f t="shared" si="23"/>
+        <v>0</v>
       </c>
       <c r="W28" s="15" t="str">
         <f t="shared" si="24"/>
@@ -5814,8 +5805,9 @@
         <f t="shared" si="25"/>
         <v>11</v>
       </c>
-      <c r="Y28" s="15" t="s">
-        <v>319</v>
+      <c r="Y28" s="10" t="str">
+        <f t="shared" si="26"/>
+        <v>00010101</v>
       </c>
       <c r="Z28" s="10" t="str">
         <f t="shared" si="27"/>
@@ -5910,7 +5902,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T29" s="17" t="str">
+      <c r="T29" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -5918,7 +5910,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="V29" s="17" t="str">
+      <c r="V29" s="25" t="str">
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
@@ -6027,7 +6019,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T30" s="17" t="str">
+      <c r="T30" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -6035,7 +6027,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V30" s="17" t="str">
+      <c r="V30" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11001</v>
       </c>
@@ -6144,7 +6136,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T31" s="17" t="str">
+      <c r="T31" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -6152,7 +6144,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V31" s="17" t="str">
+      <c r="V31" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11110</v>
       </c>
@@ -6187,7 +6179,7 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B32" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6261,7 +6253,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T32" s="17" t="str">
+      <c r="T32" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -6269,7 +6261,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V32" s="17" t="str">
+      <c r="V32" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -6378,7 +6370,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T33" s="17" t="str">
+      <c r="T33" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -6386,7 +6378,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V33" s="17" t="str">
+      <c r="V33" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11010</v>
       </c>
@@ -6495,7 +6487,7 @@
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="T34" s="17" t="str">
+      <c r="T34" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -6503,7 +6495,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V34" s="17" t="str">
+      <c r="V34" s="25" t="str">
         <f t="shared" si="23"/>
         <v>10100</v>
       </c>
@@ -6612,7 +6604,7 @@
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="T35" s="17" t="str">
+      <c r="T35" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -6620,7 +6612,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V35" s="17" t="str">
+      <c r="V35" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11011</v>
       </c>
@@ -6729,7 +6721,7 @@
         <f t="shared" si="20"/>
         <v>10</v>
       </c>
-      <c r="T36" s="17" t="str">
+      <c r="T36" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -6737,7 +6729,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V36" s="17" t="str">
+      <c r="V36" s="25" t="str">
         <f t="shared" si="23"/>
         <v>1010</v>
       </c>
@@ -6846,7 +6838,7 @@
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="T37" s="17" t="str">
+      <c r="T37" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -6854,7 +6846,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V37" s="17" t="str">
+      <c r="V37" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -6963,7 +6955,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T38" s="17" t="str">
+      <c r="T38" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -6971,7 +6963,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V38" s="17" t="str">
+      <c r="V38" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -7080,7 +7072,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T39" s="17" t="str">
+      <c r="T39" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -7088,7 +7080,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V39" s="17" t="str">
+      <c r="V39" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11100</v>
       </c>
@@ -7197,7 +7189,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T40" s="17" t="str">
+      <c r="T40" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -7205,7 +7197,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V40" s="17" t="str">
+      <c r="V40" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11101</v>
       </c>
@@ -7314,7 +7306,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T41" s="17" t="str">
+      <c r="T41" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -7322,7 +7314,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="V41" s="17" t="str">
+      <c r="V41" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11010</v>
       </c>
@@ -7431,7 +7423,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T42" s="17" t="str">
+      <c r="T42" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -7439,7 +7431,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V42" s="17" t="str">
+      <c r="V42" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -7548,7 +7540,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T43" s="17" t="str">
+      <c r="T43" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -7556,7 +7548,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="V43" s="17" t="str">
+      <c r="V43" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11010</v>
       </c>
@@ -7665,7 +7657,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T44" s="17" t="str">
+      <c r="T44" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -7673,7 +7665,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V44" s="17" t="str">
+      <c r="V44" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -7782,7 +7774,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T45" s="17" t="str">
+      <c r="T45" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -7790,7 +7782,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V45" s="17" t="str">
+      <c r="V45" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11000</v>
       </c>
@@ -7899,7 +7891,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T46" s="17" t="str">
+      <c r="T46" s="25" t="str">
         <f t="shared" si="21"/>
         <v>10</v>
       </c>
@@ -7907,7 +7899,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V46" s="17" t="str">
+      <c r="V46" s="25" t="str">
         <f t="shared" si="23"/>
         <v>1111</v>
       </c>
@@ -8016,7 +8008,7 @@
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="T47" s="17" t="str">
+      <c r="T47" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -8024,7 +8016,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V47" s="17" t="str">
+      <c r="V47" s="25" t="str">
         <f t="shared" si="23"/>
         <v>111</v>
       </c>
@@ -8133,7 +8125,7 @@
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="T48" s="17" t="str">
+      <c r="T48" s="25" t="str">
         <f t="shared" si="21"/>
         <v>10</v>
       </c>
@@ -8141,7 +8133,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V48" s="17" t="str">
+      <c r="V48" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -8250,7 +8242,7 @@
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="T49" s="17" t="str">
+      <c r="T49" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -8258,7 +8250,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V49" s="17" t="str">
+      <c r="V49" s="25" t="str">
         <f t="shared" si="23"/>
         <v>10111</v>
       </c>
@@ -8367,7 +8359,7 @@
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="T50" s="17" t="str">
+      <c r="T50" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -8375,7 +8367,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V50" s="17" t="str">
+      <c r="V50" s="25" t="str">
         <f t="shared" si="23"/>
         <v>10111</v>
       </c>
@@ -8484,7 +8476,7 @@
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="T51" s="17" t="str">
+      <c r="T51" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -8492,7 +8484,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V51" s="17" t="str">
+      <c r="V51" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11011</v>
       </c>
@@ -8601,7 +8593,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T52" s="17" t="str">
+      <c r="T52" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -8609,7 +8601,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V52" s="17" t="str">
+      <c r="V52" s="25" t="str">
         <f t="shared" si="23"/>
         <v>10111</v>
       </c>
@@ -8718,7 +8710,7 @@
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="T53" s="17" t="str">
+      <c r="T53" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -8726,7 +8718,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V53" s="17" t="str">
+      <c r="V53" s="25" t="str">
         <f t="shared" si="23"/>
         <v>10111</v>
       </c>
@@ -8835,7 +8827,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T54" s="17" t="str">
+      <c r="T54" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -8843,7 +8835,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V54" s="17" t="str">
+      <c r="V54" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -8952,7 +8944,7 @@
         <f t="shared" si="20"/>
         <v>10</v>
       </c>
-      <c r="T55" s="17" t="str">
+      <c r="T55" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -8960,7 +8952,7 @@
         <f t="shared" si="22"/>
         <v>11</v>
       </c>
-      <c r="V55" s="17" t="str">
+      <c r="V55" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -9069,7 +9061,7 @@
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="T56" s="17" t="str">
+      <c r="T56" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -9077,7 +9069,7 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="V56" s="17" t="str">
+      <c r="V56" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11010</v>
       </c>
@@ -9186,7 +9178,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T57" s="17" t="str">
+      <c r="T57" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -9194,7 +9186,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V57" s="17" t="str">
+      <c r="V57" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11001</v>
       </c>
@@ -9303,7 +9295,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T58" s="17" t="str">
+      <c r="T58" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -9311,7 +9303,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V58" s="17" t="str">
+      <c r="V58" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -9420,7 +9412,7 @@
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="T59" s="17" t="str">
+      <c r="T59" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -9428,7 +9420,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V59" s="17" t="str">
+      <c r="V59" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -9537,7 +9529,7 @@
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="T60" s="17" t="str">
+      <c r="T60" s="25" t="str">
         <f t="shared" si="21"/>
         <v>10</v>
       </c>
@@ -9545,7 +9537,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V60" s="17" t="str">
+      <c r="V60" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -9654,7 +9646,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T61" s="17" t="str">
+      <c r="T61" s="25" t="str">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -9662,7 +9654,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V61" s="17" t="str">
+      <c r="V61" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -9771,7 +9763,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T62" s="17" t="str">
+      <c r="T62" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -9779,7 +9771,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V62" s="17" t="str">
+      <c r="V62" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11000</v>
       </c>
@@ -9888,7 +9880,7 @@
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
-      <c r="T63" s="17" t="str">
+      <c r="T63" s="25" t="str">
         <f t="shared" si="21"/>
         <v>10</v>
       </c>
@@ -9896,7 +9888,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V63" s="17" t="str">
+      <c r="V63" s="25" t="str">
         <f t="shared" si="23"/>
         <v>11110</v>
       </c>
@@ -10005,7 +9997,7 @@
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="T64" s="17" t="str">
+      <c r="T64" s="25" t="str">
         <f t="shared" si="21"/>
         <v>10</v>
       </c>
@@ -10013,7 +10005,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V64" s="17" t="str">
+      <c r="V64" s="25" t="str">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -10122,7 +10114,7 @@
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="T65" s="17" t="str">
+      <c r="T65" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -10130,7 +10122,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V65" s="17" t="str">
+      <c r="V65" s="25" t="str">
         <f t="shared" si="23"/>
         <v>10111</v>
       </c>
@@ -10239,7 +10231,7 @@
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="T66" s="17" t="str">
+      <c r="T66" s="25" t="str">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
@@ -10247,7 +10239,7 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="V66" s="17" t="str">
+      <c r="V66" s="25" t="str">
         <f t="shared" si="23"/>
         <v>10111</v>
       </c>
@@ -10356,16 +10348,16 @@
         <f t="shared" ref="S67:S130" si="43">DEC2BIN(I67)</f>
         <v>11</v>
       </c>
-      <c r="T67" s="17" t="str">
-        <f t="shared" ref="T67:T130" si="44">DEC2BIN(J67)</f>
+      <c r="T67" s="25" t="str">
+        <f t="shared" ref="T67:T130" si="44">IF(ISNUMBER(SEARCH("binary", J67)),MID(J67, 8, 5),DEC2BIN(J67))</f>
         <v>1</v>
       </c>
       <c r="U67" s="17" t="str">
         <f t="shared" ref="U67:U130" si="45">DEC2BIN(K67)</f>
         <v>0</v>
       </c>
-      <c r="V67" s="17" t="str">
-        <f t="shared" ref="V67:V130" si="46">DEC2BIN(L67)</f>
+      <c r="V67" s="25" t="str">
+        <f t="shared" ref="V67:V130" si="46">IF(ISNUMBER(SEARCH("binary", L67)),MID(L67, 8, 5),DEC2BIN(L67))</f>
         <v>10111</v>
       </c>
       <c r="W67" s="15" t="str">
@@ -10473,7 +10465,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="T68" s="17" t="str">
+      <c r="T68" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -10481,7 +10473,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V68" s="17" t="str">
+      <c r="V68" s="25" t="str">
         <f t="shared" si="46"/>
         <v>10111</v>
       </c>
@@ -10590,7 +10582,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T69" s="17" t="str">
+      <c r="T69" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -10598,7 +10590,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V69" s="17" t="str">
+      <c r="V69" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -10707,7 +10699,7 @@
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
-      <c r="T70" s="17" t="str">
+      <c r="T70" s="25" t="str">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
@@ -10715,7 +10707,7 @@
         <f t="shared" si="45"/>
         <v>10100</v>
       </c>
-      <c r="V70" s="17" t="str">
+      <c r="V70" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -10824,7 +10816,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="T71" s="17" t="str">
+      <c r="T71" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -10832,7 +10824,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V71" s="17" t="str">
+      <c r="V71" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11100</v>
       </c>
@@ -10941,7 +10933,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T72" s="17" t="str">
+      <c r="T72" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -10949,7 +10941,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V72" s="17" t="str">
+      <c r="V72" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11001</v>
       </c>
@@ -11058,7 +11050,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T73" s="17" t="str">
+      <c r="T73" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -11066,7 +11058,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V73" s="17" t="str">
+      <c r="V73" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -11175,7 +11167,7 @@
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
-      <c r="T74" s="17" t="str">
+      <c r="T74" s="25" t="str">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
@@ -11183,7 +11175,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V74" s="17" t="str">
+      <c r="V74" s="25" t="str">
         <f t="shared" si="46"/>
         <v>10100</v>
       </c>
@@ -11292,7 +11284,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T75" s="17" t="str">
+      <c r="T75" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -11300,7 +11292,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V75" s="17" t="str">
+      <c r="V75" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11110</v>
       </c>
@@ -11335,7 +11327,7 @@
     </row>
     <row r="76" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B76" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11409,7 +11401,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T76" s="17" t="str">
+      <c r="T76" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -11417,7 +11409,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V76" s="17" t="str">
+      <c r="V76" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -11526,7 +11518,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T77" s="17" t="str">
+      <c r="T77" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -11534,7 +11526,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V77" s="17" t="str">
+      <c r="V77" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11010</v>
       </c>
@@ -11643,7 +11635,7 @@
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
-      <c r="T78" s="17" t="str">
+      <c r="T78" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -11651,7 +11643,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V78" s="17" t="str">
+      <c r="V78" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11110</v>
       </c>
@@ -11760,7 +11752,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="T79" s="17" t="str">
+      <c r="T79" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -11768,7 +11760,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V79" s="17" t="str">
+      <c r="V79" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11100</v>
       </c>
@@ -11877,7 +11869,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T80" s="17" t="str">
+      <c r="T80" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -11885,7 +11877,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V80" s="17" t="str">
+      <c r="V80" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11010</v>
       </c>
@@ -11994,7 +11986,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T81" s="17" t="str">
+      <c r="T81" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -12002,7 +11994,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V81" s="17" t="str">
+      <c r="V81" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -12111,7 +12103,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T82" s="17" t="str">
+      <c r="T82" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -12119,7 +12111,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V82" s="17" t="str">
+      <c r="V82" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11010</v>
       </c>
@@ -12228,7 +12220,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T83" s="17" t="str">
+      <c r="T83" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -12236,7 +12228,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V83" s="17" t="str">
+      <c r="V83" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11100</v>
       </c>
@@ -12345,7 +12337,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T84" s="17" t="str">
+      <c r="T84" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -12353,7 +12345,7 @@
         <f t="shared" si="45"/>
         <v>1</v>
       </c>
-      <c r="V84" s="17" t="str">
+      <c r="V84" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11010</v>
       </c>
@@ -12462,7 +12454,7 @@
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
-      <c r="T85" s="17" t="str">
+      <c r="T85" s="25" t="str">
         <f t="shared" si="44"/>
         <v>11</v>
       </c>
@@ -12470,7 +12462,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V85" s="17" t="str">
+      <c r="V85" s="25" t="str">
         <f t="shared" si="46"/>
         <v>111</v>
       </c>
@@ -12579,7 +12571,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T86" s="17" t="str">
+      <c r="T86" s="25" t="str">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
@@ -12587,7 +12579,7 @@
         <f t="shared" si="45"/>
         <v>1001</v>
       </c>
-      <c r="V86" s="17" t="str">
+      <c r="V86" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -12696,7 +12688,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T87" s="17" t="str">
+      <c r="T87" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -12704,7 +12696,7 @@
         <f t="shared" si="45"/>
         <v>1</v>
       </c>
-      <c r="V87" s="17" t="str">
+      <c r="V87" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11010</v>
       </c>
@@ -12813,7 +12805,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T88" s="17" t="str">
+      <c r="T88" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -12821,7 +12813,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V88" s="17" t="str">
+      <c r="V88" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11100</v>
       </c>
@@ -12930,7 +12922,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T89" s="17" t="str">
+      <c r="T89" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -12938,7 +12930,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V89" s="17" t="str">
+      <c r="V89" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11101</v>
       </c>
@@ -13047,7 +13039,7 @@
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
-      <c r="T90" s="17" t="str">
+      <c r="T90" s="25" t="str">
         <f t="shared" si="44"/>
         <v>11</v>
       </c>
@@ -13055,7 +13047,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V90" s="17" t="str">
+      <c r="V90" s="25" t="str">
         <f t="shared" si="46"/>
         <v>1100</v>
       </c>
@@ -13164,7 +13156,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T91" s="17" t="str">
+      <c r="T91" s="25" t="str">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
@@ -13172,7 +13164,7 @@
         <f t="shared" si="45"/>
         <v>1110</v>
       </c>
-      <c r="V91" s="17" t="str">
+      <c r="V91" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -13281,7 +13273,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T92" s="17" t="str">
+      <c r="T92" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -13289,7 +13281,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V92" s="17" t="str">
+      <c r="V92" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11101</v>
       </c>
@@ -13398,7 +13390,7 @@
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
-      <c r="T93" s="17" t="str">
+      <c r="T93" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -13406,7 +13398,7 @@
         <f t="shared" si="45"/>
         <v>1</v>
       </c>
-      <c r="V93" s="17" t="str">
+      <c r="V93" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11010</v>
       </c>
@@ -13515,7 +13507,7 @@
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
-      <c r="T94" s="17" t="str">
+      <c r="T94" s="25" t="str">
         <f t="shared" si="44"/>
         <v>11</v>
       </c>
@@ -13523,7 +13515,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V94" s="17" t="str">
+      <c r="V94" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -13632,7 +13624,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T95" s="17" t="str">
+      <c r="T95" s="25" t="str">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
@@ -13640,7 +13632,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V95" s="17" t="str">
+      <c r="V95" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11101</v>
       </c>
@@ -13675,7 +13667,7 @@
     </row>
     <row r="96" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A96" s="12" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B96" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13749,7 +13741,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T96" s="17" t="str">
+      <c r="T96" s="25" t="str">
         <f t="shared" si="44"/>
         <v>11110</v>
       </c>
@@ -13757,7 +13749,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V96" s="17" t="str">
+      <c r="V96" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -13792,7 +13784,7 @@
     </row>
     <row r="97" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B97" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13866,7 +13858,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T97" s="17" t="str">
+      <c r="T97" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1010</v>
       </c>
@@ -13874,7 +13866,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V97" s="17" t="str">
+      <c r="V97" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -13983,7 +13975,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T98" s="17" t="str">
+      <c r="T98" s="25" t="str">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
@@ -13991,7 +13983,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V98" s="17" t="str">
+      <c r="V98" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11101</v>
       </c>
@@ -14100,7 +14092,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T99" s="17" t="str">
+      <c r="T99" s="25" t="str">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
@@ -14108,7 +14100,7 @@
         <f t="shared" si="45"/>
         <v>11101</v>
       </c>
-      <c r="V99" s="17" t="str">
+      <c r="V99" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -14217,7 +14209,7 @@
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
-      <c r="T100" s="17" t="str">
+      <c r="T100" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -14225,7 +14217,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V100" s="17" t="str">
+      <c r="V100" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11011</v>
       </c>
@@ -14334,7 +14326,7 @@
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
-      <c r="T101" s="17" t="str">
+      <c r="T101" s="25" t="str">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
@@ -14342,7 +14334,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V101" s="17" t="str">
+      <c r="V101" s="25" t="str">
         <f t="shared" si="46"/>
         <v>1010</v>
       </c>
@@ -14451,7 +14443,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="T102" s="17" t="str">
+      <c r="T102" s="25" t="str">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
@@ -14459,7 +14451,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V102" s="17" t="str">
+      <c r="V102" s="25" t="str">
         <f t="shared" si="46"/>
         <v>1010</v>
       </c>
@@ -14568,7 +14560,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="T103" s="17" t="str">
+      <c r="T103" s="25" t="str">
         <f t="shared" si="44"/>
         <v>10</v>
       </c>
@@ -14576,7 +14568,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V103" s="17" t="str">
+      <c r="V103" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -14685,7 +14677,7 @@
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
-      <c r="T104" s="17" t="str">
+      <c r="T104" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -14693,7 +14685,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V104" s="17" t="str">
+      <c r="V104" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11010</v>
       </c>
@@ -14802,7 +14794,7 @@
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
-      <c r="T105" s="17" t="str">
+      <c r="T105" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -14810,7 +14802,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V105" s="17" t="str">
+      <c r="V105" s="25" t="str">
         <f t="shared" si="46"/>
         <v>10111</v>
       </c>
@@ -14919,7 +14911,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="T106" s="17" t="str">
+      <c r="T106" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -14927,7 +14919,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V106" s="17" t="str">
+      <c r="V106" s="25" t="str">
         <f t="shared" si="46"/>
         <v>10111</v>
       </c>
@@ -15036,7 +15028,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="T107" s="17" t="str">
+      <c r="T107" s="25" t="str">
         <f t="shared" si="44"/>
         <v>10</v>
       </c>
@@ -15044,7 +15036,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V107" s="17" t="str">
+      <c r="V107" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -15153,7 +15145,7 @@
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
-      <c r="T108" s="17" t="str">
+      <c r="T108" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -15161,7 +15153,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V108" s="17" t="str">
+      <c r="V108" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11101</v>
       </c>
@@ -15270,7 +15262,7 @@
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
-      <c r="T109" s="17" t="str">
+      <c r="T109" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -15278,7 +15270,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V109" s="17" t="str">
+      <c r="V109" s="25" t="str">
         <f t="shared" si="46"/>
         <v>10111</v>
       </c>
@@ -15387,7 +15379,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="T110" s="17" t="str">
+      <c r="T110" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -15395,7 +15387,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V110" s="17" t="str">
+      <c r="V110" s="25" t="str">
         <f t="shared" si="46"/>
         <v>10111</v>
       </c>
@@ -15504,7 +15496,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="T111" s="17" t="str">
+      <c r="T111" s="25" t="str">
         <f t="shared" si="44"/>
         <v>10</v>
       </c>
@@ -15512,7 +15504,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V111" s="17" t="str">
+      <c r="V111" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -15621,7 +15613,7 @@
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
-      <c r="T112" s="17" t="str">
+      <c r="T112" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -15629,7 +15621,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V112" s="17" t="str">
+      <c r="V112" s="25" t="str">
         <f t="shared" si="46"/>
         <v>10111</v>
       </c>
@@ -15738,7 +15730,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="T113" s="17" t="str">
+      <c r="T113" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -15746,7 +15738,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V113" s="17" t="str">
+      <c r="V113" s="25" t="str">
         <f t="shared" si="46"/>
         <v>10111</v>
       </c>
@@ -15855,7 +15847,7 @@
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
-      <c r="T114" s="17" t="str">
+      <c r="T114" s="25" t="str">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
@@ -15863,7 +15855,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V114" s="17" t="str">
+      <c r="V114" s="25" t="str">
         <f t="shared" si="46"/>
         <v>1</v>
       </c>
@@ -15972,7 +15964,7 @@
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
-      <c r="T115" s="17" t="str">
+      <c r="T115" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -15980,7 +15972,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V115" s="17" t="str">
+      <c r="V115" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11011</v>
       </c>
@@ -16089,7 +16081,7 @@
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
-      <c r="T116" s="17" t="str">
+      <c r="T116" s="25" t="str">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
@@ -16097,7 +16089,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V116" s="17" t="str">
+      <c r="V116" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -16206,7 +16198,7 @@
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
-      <c r="T117" s="17" t="str">
+      <c r="T117" s="25" t="str">
         <f t="shared" si="44"/>
         <v>11</v>
       </c>
@@ -16214,7 +16206,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V117" s="17" t="str">
+      <c r="V117" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -16323,7 +16315,7 @@
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
-      <c r="T118" s="17" t="str">
+      <c r="T118" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -16331,7 +16323,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V118" s="17" t="str">
+      <c r="V118" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -16440,7 +16432,7 @@
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
-      <c r="T119" s="17" t="str">
+      <c r="T119" s="25" t="str">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
@@ -16448,7 +16440,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V119" s="17" t="str">
+      <c r="V119" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -16557,7 +16549,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="T120" s="17" t="str">
+      <c r="T120" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -16565,7 +16557,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V120" s="17" t="str">
+      <c r="V120" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11101</v>
       </c>
@@ -16674,7 +16666,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T121" s="17" t="str">
+      <c r="T121" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -16682,7 +16674,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V121" s="17" t="str">
+      <c r="V121" s="25" t="str">
         <f t="shared" si="46"/>
         <v>10111</v>
       </c>
@@ -16791,7 +16783,7 @@
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
-      <c r="T122" s="17" t="str">
+      <c r="T122" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -16799,7 +16791,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V122" s="17" t="str">
+      <c r="V122" s="25" t="str">
         <f t="shared" si="46"/>
         <v>10111</v>
       </c>
@@ -16908,7 +16900,7 @@
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
-      <c r="T123" s="17" t="str">
+      <c r="T123" s="25" t="str">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
@@ -16916,7 +16908,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V123" s="17" t="str">
+      <c r="V123" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -17025,7 +17017,7 @@
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
-      <c r="T124" s="17" t="str">
+      <c r="T124" s="25" t="str">
         <f t="shared" si="44"/>
         <v>11</v>
       </c>
@@ -17033,7 +17025,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V124" s="17" t="str">
+      <c r="V124" s="25" t="str">
         <f t="shared" si="46"/>
         <v>110</v>
       </c>
@@ -17142,7 +17134,7 @@
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
-      <c r="T125" s="17" t="str">
+      <c r="T125" s="25" t="str">
         <f t="shared" si="44"/>
         <v>11</v>
       </c>
@@ -17150,7 +17142,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V125" s="17" t="str">
+      <c r="V125" s="25" t="str">
         <f t="shared" si="46"/>
         <v>1000</v>
       </c>
@@ -17259,7 +17251,7 @@
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
-      <c r="T126" s="17" t="str">
+      <c r="T126" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -17267,7 +17259,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V126" s="17" t="str">
+      <c r="V126" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -17376,7 +17368,7 @@
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
-      <c r="T127" s="17" t="str">
+      <c r="T127" s="25" t="str">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
@@ -17384,7 +17376,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V127" s="17" t="str">
+      <c r="V127" s="25" t="str">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
@@ -17493,7 +17485,7 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="T128" s="17" t="str">
+      <c r="T128" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -17501,7 +17493,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V128" s="17" t="str">
+      <c r="V128" s="25" t="str">
         <f t="shared" si="46"/>
         <v>11010</v>
       </c>
@@ -17610,7 +17602,7 @@
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
-      <c r="T129" s="17" t="str">
+      <c r="T129" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -17618,7 +17610,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V129" s="17" t="str">
+      <c r="V129" s="25" t="str">
         <f t="shared" si="46"/>
         <v>10111</v>
       </c>
@@ -17727,7 +17719,7 @@
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
-      <c r="T130" s="17" t="str">
+      <c r="T130" s="25" t="str">
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
@@ -17735,7 +17727,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="V130" s="17" t="str">
+      <c r="V130" s="25" t="str">
         <f t="shared" si="46"/>
         <v>10111</v>
       </c>
@@ -17844,16 +17836,16 @@
         <f t="shared" ref="S131:S146" si="66">DEC2BIN(I131)</f>
         <v>10</v>
       </c>
-      <c r="T131" s="17" t="str">
-        <f t="shared" ref="T131:T146" si="67">DEC2BIN(J131)</f>
+      <c r="T131" s="25" t="str">
+        <f t="shared" ref="T131:T146" si="67">IF(ISNUMBER(SEARCH("binary", J131)),MID(J131, 8, 5),DEC2BIN(J131))</f>
         <v>0</v>
       </c>
       <c r="U131" s="17" t="str">
         <f t="shared" ref="U131:U146" si="68">DEC2BIN(K131)</f>
         <v>0</v>
       </c>
-      <c r="V131" s="17" t="str">
-        <f t="shared" ref="V131:V146" si="69">DEC2BIN(L131)</f>
+      <c r="V131" s="25" t="str">
+        <f t="shared" ref="V131:V146" si="69">IF(ISNUMBER(SEARCH("binary", L131)),MID(L131, 8, 5),DEC2BIN(L131))</f>
         <v>0</v>
       </c>
       <c r="W131" s="15" t="str">
@@ -17961,7 +17953,7 @@
         <f t="shared" si="66"/>
         <v>1</v>
       </c>
-      <c r="T132" s="17" t="str">
+      <c r="T132" s="25" t="str">
         <f t="shared" si="67"/>
         <v>11</v>
       </c>
@@ -17969,7 +17961,7 @@
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
-      <c r="V132" s="17" t="str">
+      <c r="V132" s="25" t="str">
         <f t="shared" si="69"/>
         <v>1110</v>
       </c>
@@ -18078,7 +18070,7 @@
         <f t="shared" si="66"/>
         <v>10</v>
       </c>
-      <c r="T133" s="17" t="str">
+      <c r="T133" s="25" t="str">
         <f t="shared" si="67"/>
         <v>11</v>
       </c>
@@ -18086,7 +18078,7 @@
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
-      <c r="V133" s="17" t="str">
+      <c r="V133" s="25" t="str">
         <f t="shared" si="69"/>
         <v>10000</v>
       </c>
@@ -18195,7 +18187,7 @@
         <f t="shared" si="66"/>
         <v>10</v>
       </c>
-      <c r="T134" s="17" t="str">
+      <c r="T134" s="25" t="str">
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
@@ -18203,7 +18195,7 @@
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
-      <c r="V134" s="17" t="str">
+      <c r="V134" s="25" t="str">
         <f t="shared" si="69"/>
         <v>0</v>
       </c>
@@ -18312,7 +18304,7 @@
         <f t="shared" si="66"/>
         <v>1</v>
       </c>
-      <c r="T135" s="17" t="str">
+      <c r="T135" s="25" t="str">
         <f t="shared" si="67"/>
         <v>0</v>
       </c>
@@ -18320,7 +18312,7 @@
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
-      <c r="V135" s="17" t="str">
+      <c r="V135" s="25" t="str">
         <f t="shared" si="69"/>
         <v>0</v>
       </c>
@@ -18429,7 +18421,7 @@
         <f t="shared" si="66"/>
         <v>10</v>
       </c>
-      <c r="T136" s="17" t="str">
+      <c r="T136" s="25" t="str">
         <f t="shared" si="67"/>
         <v>0</v>
       </c>
@@ -18437,7 +18429,7 @@
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
-      <c r="V136" s="17" t="str">
+      <c r="V136" s="25" t="str">
         <f t="shared" si="69"/>
         <v>1010</v>
       </c>
@@ -18546,7 +18538,7 @@
         <f t="shared" si="66"/>
         <v>11</v>
       </c>
-      <c r="T137" s="17" t="str">
+      <c r="T137" s="25" t="str">
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
@@ -18554,7 +18546,7 @@
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
-      <c r="V137" s="17" t="str">
+      <c r="V137" s="25" t="str">
         <f t="shared" si="69"/>
         <v>10111</v>
       </c>
@@ -18663,7 +18655,7 @@
         <f t="shared" si="66"/>
         <v>10</v>
       </c>
-      <c r="T138" s="17" t="str">
+      <c r="T138" s="25" t="str">
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
@@ -18671,7 +18663,7 @@
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
-      <c r="V138" s="17" t="str">
+      <c r="V138" s="25" t="str">
         <f t="shared" si="69"/>
         <v>10111</v>
       </c>
@@ -18780,7 +18772,7 @@
         <f t="shared" si="66"/>
         <v>10</v>
       </c>
-      <c r="T139" s="17" t="str">
+      <c r="T139" s="25" t="str">
         <f t="shared" si="67"/>
         <v>0</v>
       </c>
@@ -18788,7 +18780,7 @@
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
-      <c r="V139" s="17" t="str">
+      <c r="V139" s="25" t="str">
         <f t="shared" si="69"/>
         <v>0</v>
       </c>
@@ -18897,7 +18889,7 @@
         <f t="shared" si="66"/>
         <v>1</v>
       </c>
-      <c r="T140" s="17" t="str">
+      <c r="T140" s="25" t="str">
         <f t="shared" si="67"/>
         <v>11</v>
       </c>
@@ -18905,7 +18897,7 @@
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
-      <c r="V140" s="17" t="str">
+      <c r="V140" s="25" t="str">
         <f t="shared" si="69"/>
         <v>10110</v>
       </c>
@@ -19014,15 +19006,16 @@
         <f t="shared" si="66"/>
         <v>10</v>
       </c>
-      <c r="T141" s="17" t="str">
+      <c r="T141" s="25" t="str">
         <f t="shared" si="67"/>
         <v>11</v>
       </c>
       <c r="U141" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="V141" s="17" t="s">
-        <v>317</v>
+      <c r="V141" s="25" t="str">
+        <f t="shared" si="69"/>
+        <v>0</v>
       </c>
       <c r="W141" s="15" t="str">
         <f t="shared" si="70"/>
@@ -19042,11 +19035,11 @@
       </c>
       <c r="AA141" s="10" t="str">
         <f t="shared" si="74"/>
-        <v>10111</v>
+        <v>00000</v>
       </c>
       <c r="AB141" s="11" t="str">
         <f t="shared" si="75"/>
-        <v>0010001011010111</v>
+        <v>0010001011000000</v>
       </c>
       <c r="AC141" s="10">
         <f t="shared" si="76"/>
@@ -19129,7 +19122,7 @@
         <f t="shared" si="66"/>
         <v>10</v>
       </c>
-      <c r="T142" s="17" t="str">
+      <c r="T142" s="25" t="str">
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
@@ -19137,7 +19130,7 @@
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
-      <c r="V142" s="17" t="str">
+      <c r="V142" s="25" t="str">
         <f t="shared" si="69"/>
         <v>0</v>
       </c>
@@ -19246,7 +19239,7 @@
         <f t="shared" si="66"/>
         <v>11</v>
       </c>
-      <c r="T143" s="17" t="str">
+      <c r="T143" s="25" t="str">
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
@@ -19254,7 +19247,7 @@
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
-      <c r="V143" s="17" t="str">
+      <c r="V143" s="25" t="str">
         <f t="shared" si="69"/>
         <v>0</v>
       </c>
@@ -19363,7 +19356,7 @@
         <f t="shared" si="66"/>
         <v>11</v>
       </c>
-      <c r="T144" s="17" t="str">
+      <c r="T144" s="25" t="str">
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
@@ -19371,7 +19364,7 @@
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
-      <c r="V144" s="17" t="str">
+      <c r="V144" s="25" t="str">
         <f t="shared" si="69"/>
         <v>11001</v>
       </c>
@@ -19480,7 +19473,7 @@
         <f t="shared" si="66"/>
         <v>11</v>
       </c>
-      <c r="T145" s="17" t="str">
+      <c r="T145" s="25" t="str">
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
@@ -19488,7 +19481,7 @@
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
-      <c r="V145" s="17" t="str">
+      <c r="V145" s="25" t="str">
         <f t="shared" si="69"/>
         <v>0</v>
       </c>
@@ -19597,7 +19590,7 @@
         <f t="shared" si="66"/>
         <v>0</v>
       </c>
-      <c r="T146" s="17" t="str">
+      <c r="T146" s="25" t="str">
         <f t="shared" si="67"/>
         <v>0</v>
       </c>
@@ -19605,7 +19598,7 @@
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
-      <c r="V146" s="17" t="str">
+      <c r="V146" s="25" t="str">
         <f t="shared" si="69"/>
         <v>0</v>
       </c>
@@ -20254,6 +20247,9 @@
   <autoFilter ref="A1:AC146"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="T2:T146" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added conditional formatting so cell is red if bit instruction is not 16 bits
</commit_message>
<xml_diff>
--- a/Convert to Binary_v3 - Program 1.xlsx
+++ b/Convert to Binary_v3 - Program 1.xlsx
@@ -1188,7 +1188,29 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -2558,7 +2580,7 @@
   <dimension ref="A1:AD248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AC2" sqref="AC2"/>
@@ -2780,7 +2802,7 @@
         <v>0000111100000101</v>
       </c>
       <c r="AC2" s="10">
-        <f t="shared" ref="AC2" si="7">LEN(AB2)</f>
+        <f t="shared" ref="AC2:AC65" si="7">LEN(AB2)</f>
         <v>16</v>
       </c>
     </row>
@@ -2897,7 +2919,7 @@
         <v>0110011111000101</v>
       </c>
       <c r="AC3" s="10">
-        <f t="shared" ref="AC3:AC66" si="30">LEN(AB3)</f>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -3014,7 +3036,7 @@
         <v>0001101100000000</v>
       </c>
       <c r="AC4" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -3131,7 +3153,7 @@
         <v>0000101100011101</v>
       </c>
       <c r="AC5" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -3248,7 +3270,7 @@
         <v>1000010001011101</v>
       </c>
       <c r="AC6" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -3365,7 +3387,7 @@
         <v>0000111100011110</v>
       </c>
       <c r="AC7" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -3482,7 +3504,7 @@
         <v>0001101100011110</v>
       </c>
       <c r="AC8" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -3599,7 +3621,7 @@
         <v>0001101100001001</v>
       </c>
       <c r="AC9" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -3716,7 +3738,7 @@
         <v>0000101100011101</v>
       </c>
       <c r="AC10" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -3833,7 +3855,7 @@
         <v>1000010010011101</v>
       </c>
       <c r="AC11" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -3950,7 +3972,7 @@
         <v>0001101100011110</v>
       </c>
       <c r="AC12" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -4067,7 +4089,7 @@
         <v>0001101100001001</v>
       </c>
       <c r="AC13" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -4184,7 +4206,7 @@
         <v>0000101100011101</v>
       </c>
       <c r="AC14" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -4301,7 +4323,7 @@
         <v>1000010011011101</v>
       </c>
       <c r="AC15" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -4418,7 +4440,7 @@
         <v>0000111100011111</v>
       </c>
       <c r="AC16" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -4535,7 +4557,7 @@
         <v>0110011111000101</v>
       </c>
       <c r="AC17" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -4652,7 +4674,7 @@
         <v>0001101100011111</v>
       </c>
       <c r="AC18" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -4769,7 +4791,7 @@
         <v>0110011111000101</v>
       </c>
       <c r="AC19" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -4886,7 +4908,7 @@
         <v>0001101100011111</v>
       </c>
       <c r="AC20" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -5003,7 +5025,7 @@
         <v>0110011111000001</v>
       </c>
       <c r="AC21" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -5120,7 +5142,7 @@
         <v>0001101100000001</v>
       </c>
       <c r="AC22" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -5237,7 +5259,7 @@
         <v>0000101101011000</v>
       </c>
       <c r="AC23" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -5354,7 +5376,7 @@
         <v>0000111100010101</v>
       </c>
       <c r="AC24" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -5471,7 +5493,7 @@
         <v>0110011111000101</v>
       </c>
       <c r="AC25" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -5588,7 +5610,7 @@
         <v>0001101100001010</v>
       </c>
       <c r="AC26" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -5705,7 +5727,7 @@
         <v>0110011111000101</v>
       </c>
       <c r="AC27" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -5822,7 +5844,7 @@
         <v>0001101100010101</v>
       </c>
       <c r="AC28" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -5939,7 +5961,7 @@
         <v>0110011111000001</v>
       </c>
       <c r="AC29" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -6056,7 +6078,7 @@
         <v>0000101101011001</v>
       </c>
       <c r="AC30" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -6173,7 +6195,7 @@
         <v>0000111101011110</v>
       </c>
       <c r="AC31" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -6290,7 +6312,7 @@
         <v>0001111100000001</v>
       </c>
       <c r="AC32" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -6407,7 +6429,7 @@
         <v>0000101101011010</v>
       </c>
       <c r="AC33" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -6524,7 +6546,7 @@
         <v>0000110100010100</v>
       </c>
       <c r="AC34" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -6641,7 +6663,7 @@
         <v>0000100101011011</v>
       </c>
       <c r="AC35" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -6758,7 +6780,7 @@
         <v>0000111000001010</v>
       </c>
       <c r="AC36" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -6875,7 +6897,7 @@
         <v>0000110000000000</v>
       </c>
       <c r="AC37" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -6992,7 +7014,7 @@
         <v>0000111100000000</v>
       </c>
       <c r="AC38" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -7109,7 +7131,7 @@
         <v>0000101101011100</v>
       </c>
       <c r="AC39" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -7226,7 +7248,7 @@
         <v>0000101101011101</v>
       </c>
       <c r="AC40" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -7343,7 +7365,7 @@
         <v>0000011101111010</v>
       </c>
       <c r="AC41" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -7460,7 +7482,7 @@
         <v>0001101100000001</v>
       </c>
       <c r="AC42" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -7577,7 +7599,7 @@
         <v>0000101101111010</v>
       </c>
       <c r="AC43" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -7694,7 +7716,7 @@
         <v>1100011100000000</v>
       </c>
       <c r="AC44" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -7811,7 +7833,7 @@
         <v>0001011101011000</v>
       </c>
       <c r="AC45" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -7928,7 +7950,7 @@
         <v>0010001110001111</v>
       </c>
       <c r="AC46" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -8045,7 +8067,7 @@
         <v>0000100101000111</v>
       </c>
       <c r="AC47" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -8162,7 +8184,7 @@
         <v>0100000010000000</v>
       </c>
       <c r="AC48" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -8279,7 +8301,7 @@
         <v>0000100101010111</v>
       </c>
       <c r="AC49" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -8396,7 +8418,7 @@
         <v>0000010001010111</v>
       </c>
       <c r="AC50" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -8513,7 +8535,7 @@
         <v>0000010101011011</v>
       </c>
       <c r="AC51" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -8630,7 +8652,7 @@
         <v>0000101101010111</v>
       </c>
       <c r="AC52" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -8747,7 +8769,7 @@
         <v>0001000001010111</v>
       </c>
       <c r="AC53" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -8864,7 +8886,7 @@
         <v>1100101100000001</v>
       </c>
       <c r="AC54" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -8981,7 +9003,7 @@
         <v>0010110010000011</v>
       </c>
       <c r="AC55" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -9098,7 +9120,7 @@
         <v>0000100001111010</v>
       </c>
       <c r="AC56" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -9215,7 +9237,7 @@
         <v>0000011101011001</v>
       </c>
       <c r="AC57" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -9332,7 +9354,7 @@
         <v>1100101100000001</v>
       </c>
       <c r="AC58" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -9449,7 +9471,7 @@
         <v>0000110000000000</v>
       </c>
       <c r="AC59" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -9566,7 +9588,7 @@
         <v>0011100110000000</v>
       </c>
       <c r="AC60" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -9683,7 +9705,7 @@
         <v>1100011100000000</v>
       </c>
       <c r="AC61" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -9800,7 +9822,7 @@
         <v>0001011101011000</v>
       </c>
       <c r="AC62" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -9917,7 +9939,7 @@
         <v>0010001110011110</v>
       </c>
       <c r="AC63" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -10034,7 +10056,7 @@
         <v>0100000010000000</v>
       </c>
       <c r="AC64" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -10151,7 +10173,7 @@
         <v>0000100101010111</v>
       </c>
       <c r="AC65" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -10268,7 +10290,7 @@
         <v>0000010001010111</v>
       </c>
       <c r="AC66" s="10">
-        <f t="shared" si="30"/>
+        <f t="shared" ref="AC66:AC129" si="30">LEN(AB66)</f>
         <v>16</v>
       </c>
     </row>
@@ -10385,7 +10407,7 @@
         <v>0000101101010111</v>
       </c>
       <c r="AC67" s="10">
-        <f t="shared" ref="AC67:AC130" si="53">LEN(AB67)</f>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -10502,7 +10524,7 @@
         <v>0001000001010111</v>
       </c>
       <c r="AC68" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -10619,7 +10641,7 @@
         <v>1100101100000001</v>
       </c>
       <c r="AC69" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -10736,7 +10758,7 @@
         <v>0010110010010100</v>
       </c>
       <c r="AC70" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -10853,7 +10875,7 @@
         <v>0000100001011100</v>
       </c>
       <c r="AC71" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -10970,7 +10992,7 @@
         <v>0000011101011001</v>
       </c>
       <c r="AC72" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -11087,7 +11109,7 @@
         <v>1100101100000001</v>
       </c>
       <c r="AC73" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -11204,7 +11226,7 @@
         <v>0000110100010100</v>
       </c>
       <c r="AC74" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -11321,7 +11343,7 @@
         <v>0000111101011110</v>
       </c>
       <c r="AC75" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -11438,7 +11460,7 @@
         <v>0001111100000001</v>
       </c>
       <c r="AC76" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -11555,7 +11577,7 @@
         <v>0000101101011010</v>
       </c>
       <c r="AC77" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -11672,7 +11694,7 @@
         <v>0000011001011110</v>
       </c>
       <c r="AC78" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -11789,7 +11811,7 @@
         <v>0000010001011100</v>
       </c>
       <c r="AC79" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -11906,7 +11928,7 @@
         <v>0000011101011010</v>
       </c>
       <c r="AC80" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -12023,7 +12045,7 @@
         <v>0001101100000001</v>
       </c>
       <c r="AC81" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -12140,7 +12162,7 @@
         <v>0000101101011010</v>
       </c>
       <c r="AC82" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -12257,7 +12279,7 @@
         <v>0000011101011100</v>
       </c>
       <c r="AC83" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -12374,7 +12396,7 @@
         <v>0001011101111010</v>
       </c>
       <c r="AC84" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -12491,7 +12513,7 @@
         <v>0010100111000111</v>
       </c>
       <c r="AC85" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -12608,7 +12630,7 @@
         <v>0010110011001001</v>
       </c>
       <c r="AC86" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -12725,7 +12747,7 @@
         <v>0000011101111010</v>
       </c>
       <c r="AC87" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -12842,7 +12864,7 @@
         <v>0001011101011100</v>
       </c>
       <c r="AC88" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -12959,7 +12981,7 @@
         <v>0001011101011101</v>
       </c>
       <c r="AC89" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -13076,7 +13098,7 @@
         <v>0010100111001100</v>
       </c>
       <c r="AC90" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -13193,7 +13215,7 @@
         <v>0010110011001110</v>
       </c>
       <c r="AC91" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -13310,7 +13332,7 @@
         <v>0000101101011101</v>
       </c>
       <c r="AC92" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -13427,7 +13449,7 @@
         <v>0000011001111010</v>
       </c>
       <c r="AC93" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -13544,7 +13566,7 @@
         <v>0011100111000000</v>
       </c>
       <c r="AC94" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -13661,7 +13683,7 @@
         <v>0000111100011101</v>
       </c>
       <c r="AC95" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -13778,7 +13800,7 @@
         <v>0001101100011110</v>
       </c>
       <c r="AC96" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -13895,7 +13917,7 @@
         <v>0001101100001010</v>
       </c>
       <c r="AC97" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -14012,7 +14034,7 @@
         <v>0000101100011101</v>
       </c>
       <c r="AC98" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -14129,7 +14151,7 @@
         <v>1000010011011101</v>
       </c>
       <c r="AC99" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -14246,7 +14268,7 @@
         <v>0000101001011011</v>
       </c>
       <c r="AC100" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -14363,7 +14385,7 @@
         <v>0000111000001010</v>
       </c>
       <c r="AC101" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -14480,7 +14502,7 @@
         <v>0000110000001010</v>
       </c>
       <c r="AC102" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -14597,7 +14619,7 @@
         <v>0100000010000000</v>
       </c>
       <c r="AC103" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -14714,7 +14736,7 @@
         <v>0000010101011010</v>
       </c>
       <c r="AC104" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -14831,7 +14853,7 @@
         <v>0000100101010111</v>
       </c>
       <c r="AC105" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -14948,7 +14970,7 @@
         <v>0000010001010111</v>
       </c>
       <c r="AC106" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -15065,7 +15087,7 @@
         <v>0100000010000000</v>
       </c>
       <c r="AC107" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -15182,7 +15204,7 @@
         <v>0000010101011101</v>
       </c>
       <c r="AC108" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -15299,7 +15321,7 @@
         <v>0000100101010111</v>
       </c>
       <c r="AC109" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -15416,7 +15438,7 @@
         <v>0000010001010111</v>
       </c>
       <c r="AC110" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -15533,7 +15555,7 @@
         <v>0100000010000000</v>
       </c>
       <c r="AC111" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -15650,7 +15672,7 @@
         <v>0000100101010111</v>
       </c>
       <c r="AC112" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -15767,7 +15789,7 @@
         <v>0000010001010111</v>
       </c>
       <c r="AC113" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -15884,7 +15906,7 @@
         <v>0000110100000001</v>
       </c>
       <c r="AC114" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -16001,7 +16023,7 @@
         <v>0000011001011011</v>
       </c>
       <c r="AC115" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -16118,7 +16140,7 @@
         <v>0100011000000000</v>
       </c>
       <c r="AC116" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -16235,7 +16257,7 @@
         <v>0010001011000000</v>
       </c>
       <c r="AC117" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -16352,7 +16374,7 @@
         <v>1100101000000001</v>
       </c>
       <c r="AC118" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -16469,7 +16491,7 @@
         <v>0000110100000000</v>
       </c>
       <c r="AC119" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -16586,7 +16608,7 @@
         <v>0000110001011101</v>
       </c>
       <c r="AC120" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -16703,7 +16725,7 @@
         <v>0000101101010111</v>
       </c>
       <c r="AC121" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -16820,7 +16842,7 @@
         <v>0000011001010111</v>
       </c>
       <c r="AC122" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -16937,7 +16959,7 @@
         <v>0100011000000000</v>
       </c>
       <c r="AC123" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -17054,7 +17076,7 @@
         <v>0010000111000110</v>
       </c>
       <c r="AC124" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -17171,7 +17193,7 @@
         <v>0010001011001000</v>
       </c>
       <c r="AC125" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -17288,7 +17310,7 @@
         <v>1100101000000001</v>
       </c>
       <c r="AC126" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -17405,7 +17427,7 @@
         <v>0000110100000000</v>
       </c>
       <c r="AC127" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -17522,7 +17544,7 @@
         <v>0000010001011010</v>
       </c>
       <c r="AC128" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -17639,7 +17661,7 @@
         <v>0000101101010111</v>
       </c>
       <c r="AC129" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="30"/>
         <v>16</v>
       </c>
     </row>
@@ -17756,7 +17778,7 @@
         <v>0000011001010111</v>
       </c>
       <c r="AC130" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" ref="AC130:AC146" si="53">LEN(AB130)</f>
         <v>16</v>
       </c>
     </row>
@@ -17873,7 +17895,7 @@
         <v>0100011000000000</v>
       </c>
       <c r="AC131" s="10">
-        <f t="shared" ref="AC131:AC146" si="76">LEN(AB131)</f>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -17990,7 +18012,7 @@
         <v>0010000111001110</v>
       </c>
       <c r="AC132" s="10">
-        <f t="shared" si="76"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -18107,7 +18129,7 @@
         <v>0010001011010000</v>
       </c>
       <c r="AC133" s="10">
-        <f t="shared" si="76"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -18224,7 +18246,7 @@
         <v>1100101000000001</v>
       </c>
       <c r="AC134" s="10">
-        <f t="shared" si="76"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -18341,7 +18363,7 @@
         <v>0000110100000000</v>
       </c>
       <c r="AC135" s="10">
-        <f t="shared" si="76"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -18458,7 +18480,7 @@
         <v>0000111000001010</v>
       </c>
       <c r="AC136" s="10">
-        <f t="shared" si="76"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -18575,7 +18597,7 @@
         <v>0000101101010111</v>
       </c>
       <c r="AC137" s="10">
-        <f t="shared" si="76"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -18692,7 +18714,7 @@
         <v>0000011001010111</v>
       </c>
       <c r="AC138" s="10">
-        <f t="shared" si="76"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -18809,7 +18831,7 @@
         <v>0100011000000000</v>
       </c>
       <c r="AC139" s="10">
-        <f t="shared" si="76"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -18926,7 +18948,7 @@
         <v>0010000111010110</v>
       </c>
       <c r="AC140" s="10">
-        <f t="shared" si="76"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -19042,7 +19064,7 @@
         <v>0010001011000000</v>
       </c>
       <c r="AC141" s="10">
-        <f t="shared" si="76"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -19159,7 +19181,7 @@
         <v>1100101000000001</v>
       </c>
       <c r="AC142" s="10">
-        <f t="shared" si="76"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -19276,7 +19298,7 @@
         <v>1100101100000001</v>
       </c>
       <c r="AC143" s="10">
-        <f t="shared" si="76"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -19393,7 +19415,7 @@
         <v>0000011101011001</v>
       </c>
       <c r="AC144" s="10">
-        <f t="shared" si="76"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -19510,7 +19532,7 @@
         <v>1100101100000001</v>
       </c>
       <c r="AC145" s="10">
-        <f t="shared" si="76"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -19627,7 +19649,7 @@
         <v>0000000000000000</v>
       </c>
       <c r="AC146" s="10">
-        <f t="shared" si="76"/>
+        <f t="shared" si="53"/>
         <v>16</v>
       </c>
     </row>
@@ -20245,6 +20267,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AC146"/>
+  <conditionalFormatting sqref="AC2:AC146">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="notEqual">
+      <formula>16</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
debugging Program 1 (ongoing)
</commit_message>
<xml_diff>
--- a/Convert to Binary_v3 - Program 1.xlsx
+++ b/Convert to Binary_v3 - Program 1.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="313">
   <si>
     <t>LDX 1,0,29</t>
   </si>
@@ -928,9 +928,6 @@
     <t>If R1 = 0 (no more leading zeros), jump to PRINT TENS PLACE</t>
   </si>
   <si>
-    <t>JZ 2,3,23(g1p)</t>
-  </si>
-  <si>
     <t>If the quotient (in R2) = 0, jump to PRINT ONES PLACE</t>
   </si>
   <si>
@@ -968,6 +965,9 @@
   </si>
   <si>
     <t>AIR 3,10</t>
+  </si>
+  <si>
+    <t>JZ 2,3,0,23(g1p)</t>
   </si>
 </sst>
 </file>
@@ -1494,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H145"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
-      <selection sqref="A1:A145"/>
+    <sheetView topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1547,12 +1547,12 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1570,7 +1570,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F11" t="s">
         <v>148</v>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1612,7 +1612,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D17" t="s">
         <v>153</v>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D19" t="s">
         <v>154</v>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F21" t="s">
         <v>156</v>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C23" t="s">
         <v>159</v>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1680,7 +1680,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1709,7 +1709,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -2037,7 +2037,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -2191,7 +2191,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F95" t="s">
         <v>254</v>
@@ -2199,7 +2199,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -2527,10 +2527,10 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
+        <v>312</v>
+      </c>
+      <c r="E140" t="s">
         <v>299</v>
-      </c>
-      <c r="E140" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
@@ -2538,7 +2538,7 @@
         <v>274</v>
       </c>
       <c r="G141" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
@@ -2546,7 +2546,7 @@
         <v>200</v>
       </c>
       <c r="G142" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
@@ -2567,7 +2567,7 @@
         <v>13</v>
       </c>
       <c r="H145" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -2580,10 +2580,10 @@
   <dimension ref="A1:AD248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC2" sqref="AC2"/>
+      <selection pane="bottomRight" activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2761,20 +2761,20 @@
         <f t="shared" ref="R2" si="2">M2</f>
         <v>000011</v>
       </c>
-      <c r="S2" s="17" t="str">
-        <f t="shared" ref="S2:U2" si="3">DEC2BIN(I2)</f>
+      <c r="S2" s="25" t="str">
+        <f>IF(ISNUMBER(SEARCH("binary", I2)),MID(I2, 8, 5),DEC2BIN(I2))</f>
         <v>11</v>
       </c>
       <c r="T2" s="25" t="str">
-        <f>IF(ISNUMBER(SEARCH("binary", J2)),MID(J2, 8, 5),DEC2BIN(J2))</f>
-        <v>0</v>
-      </c>
-      <c r="U2" s="17" t="str">
+        <f t="shared" ref="T2:V2" si="3">IF(ISNUMBER(SEARCH("binary", J2)),MID(J2, 8, 5),DEC2BIN(J2))</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="25" t="str">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V2" s="25" t="str">
-        <f>IF(ISNUMBER(SEARCH("binary", L2)),MID(L2, 8, 5),DEC2BIN(L2))</f>
+        <f t="shared" si="3"/>
         <v>101</v>
       </c>
       <c r="W2" s="15" t="str">
@@ -2878,16 +2878,16 @@
         <f t="shared" ref="R3:R66" si="19">M3</f>
         <v>011001</v>
       </c>
-      <c r="S3" s="17" t="str">
-        <f t="shared" ref="S3:S66" si="20">DEC2BIN(I3)</f>
+      <c r="S3" s="25" t="str">
+        <f t="shared" ref="S3:S66" si="20">IF(ISNUMBER(SEARCH("binary", I3)),MID(I3, 8, 5),DEC2BIN(I3))</f>
         <v>11</v>
       </c>
       <c r="T3" s="25" t="str">
         <f t="shared" ref="T3:T66" si="21">IF(ISNUMBER(SEARCH("binary", J3)),MID(J3, 8, 5),DEC2BIN(J3))</f>
         <v>1</v>
       </c>
-      <c r="U3" s="17" t="str">
-        <f t="shared" ref="U3:U66" si="22">DEC2BIN(K3)</f>
+      <c r="U3" s="25" t="str">
+        <f t="shared" ref="U3:U66" si="22">IF(ISNUMBER(SEARCH("binary", K3)),MID(K3, 8, 5),DEC2BIN(K3))</f>
         <v>1</v>
       </c>
       <c r="V3" s="25" t="str">
@@ -2995,7 +2995,7 @@
         <f t="shared" si="19"/>
         <v>000110</v>
       </c>
-      <c r="S4" s="17" t="str">
+      <c r="S4" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -3003,7 +3003,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U4" s="17" t="str">
+      <c r="U4" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -3112,7 +3112,7 @@
         <f t="shared" si="19"/>
         <v>000010</v>
       </c>
-      <c r="S5" s="17" t="str">
+      <c r="S5" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -3120,7 +3120,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U5" s="17" t="str">
+      <c r="U5" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -3229,7 +3229,7 @@
         <f t="shared" si="19"/>
         <v>100001</v>
       </c>
-      <c r="S6" s="17" t="str">
+      <c r="S6" s="25" t="str">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
@@ -3237,7 +3237,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U6" s="17" t="str">
+      <c r="U6" s="25" t="str">
         <f t="shared" si="22"/>
         <v>11101</v>
       </c>
@@ -3346,7 +3346,7 @@
         <f t="shared" si="19"/>
         <v>000011</v>
       </c>
-      <c r="S7" s="17" t="str">
+      <c r="S7" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -3354,7 +3354,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U7" s="17" t="str">
+      <c r="U7" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -3393,7 +3393,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B8" s="9" t="str">
         <f t="shared" si="8"/>
@@ -3463,7 +3463,7 @@
         <f t="shared" si="19"/>
         <v>000110</v>
       </c>
-      <c r="S8" s="17" t="str">
+      <c r="S8" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -3471,7 +3471,7 @@
         <f t="shared" si="21"/>
         <v>11110</v>
       </c>
-      <c r="U8" s="17" t="str">
+      <c r="U8" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -3510,7 +3510,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B9" s="9" t="str">
         <f t="shared" si="8"/>
@@ -3580,7 +3580,7 @@
         <f t="shared" si="19"/>
         <v>000110</v>
       </c>
-      <c r="S9" s="17" t="str">
+      <c r="S9" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -3588,7 +3588,7 @@
         <f t="shared" si="21"/>
         <v>1001</v>
       </c>
-      <c r="U9" s="17" t="str">
+      <c r="U9" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -3697,7 +3697,7 @@
         <f t="shared" si="19"/>
         <v>000010</v>
       </c>
-      <c r="S10" s="17" t="str">
+      <c r="S10" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -3705,7 +3705,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U10" s="17" t="str">
+      <c r="U10" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -3814,7 +3814,7 @@
         <f t="shared" si="19"/>
         <v>100001</v>
       </c>
-      <c r="S11" s="17" t="str">
+      <c r="S11" s="25" t="str">
         <f t="shared" si="20"/>
         <v>10</v>
       </c>
@@ -3822,7 +3822,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U11" s="17" t="str">
+      <c r="U11" s="25" t="str">
         <f t="shared" si="22"/>
         <v>11101</v>
       </c>
@@ -3861,7 +3861,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B12" s="9" t="str">
         <f t="shared" si="8"/>
@@ -3931,7 +3931,7 @@
         <f t="shared" si="19"/>
         <v>000110</v>
       </c>
-      <c r="S12" s="17" t="str">
+      <c r="S12" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -3939,7 +3939,7 @@
         <f t="shared" si="21"/>
         <v>11110</v>
       </c>
-      <c r="U12" s="17" t="str">
+      <c r="U12" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -3978,7 +3978,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B13" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4048,7 +4048,7 @@
         <f t="shared" si="19"/>
         <v>000110</v>
       </c>
-      <c r="S13" s="17" t="str">
+      <c r="S13" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -4056,7 +4056,7 @@
         <f t="shared" si="21"/>
         <v>1001</v>
       </c>
-      <c r="U13" s="17" t="str">
+      <c r="U13" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -4165,7 +4165,7 @@
         <f t="shared" si="19"/>
         <v>000010</v>
       </c>
-      <c r="S14" s="17" t="str">
+      <c r="S14" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -4173,7 +4173,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U14" s="17" t="str">
+      <c r="U14" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -4282,7 +4282,7 @@
         <f t="shared" si="19"/>
         <v>100001</v>
       </c>
-      <c r="S15" s="17" t="str">
+      <c r="S15" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -4290,7 +4290,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U15" s="17" t="str">
+      <c r="U15" s="25" t="str">
         <f t="shared" si="22"/>
         <v>11101</v>
       </c>
@@ -4399,7 +4399,7 @@
         <f t="shared" si="19"/>
         <v>000011</v>
       </c>
-      <c r="S16" s="17" t="str">
+      <c r="S16" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -4407,7 +4407,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U16" s="17" t="str">
+      <c r="U16" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -4516,7 +4516,7 @@
         <f t="shared" si="19"/>
         <v>011001</v>
       </c>
-      <c r="S17" s="17" t="str">
+      <c r="S17" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -4524,7 +4524,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U17" s="17" t="str">
+      <c r="U17" s="25" t="str">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
@@ -4563,7 +4563,7 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B18" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4633,7 +4633,7 @@
         <f t="shared" si="19"/>
         <v>000110</v>
       </c>
-      <c r="S18" s="17" t="str">
+      <c r="S18" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -4641,7 +4641,7 @@
         <f t="shared" si="21"/>
         <v>11111</v>
       </c>
-      <c r="U18" s="17" t="str">
+      <c r="U18" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -4750,7 +4750,7 @@
         <f t="shared" si="19"/>
         <v>011001</v>
       </c>
-      <c r="S19" s="17" t="str">
+      <c r="S19" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -4758,7 +4758,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U19" s="17" t="str">
+      <c r="U19" s="25" t="str">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
@@ -4797,7 +4797,7 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B20" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4867,7 +4867,7 @@
         <f t="shared" si="19"/>
         <v>000110</v>
       </c>
-      <c r="S20" s="17" t="str">
+      <c r="S20" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -4875,7 +4875,7 @@
         <f t="shared" si="21"/>
         <v>11111</v>
       </c>
-      <c r="U20" s="17" t="str">
+      <c r="U20" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -4984,7 +4984,7 @@
         <f t="shared" si="19"/>
         <v>011001</v>
       </c>
-      <c r="S21" s="17" t="str">
+      <c r="S21" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -4992,7 +4992,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U21" s="17" t="str">
+      <c r="U21" s="25" t="str">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
@@ -5031,7 +5031,7 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B22" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5101,7 +5101,7 @@
         <f t="shared" si="19"/>
         <v>000110</v>
       </c>
-      <c r="S22" s="17" t="str">
+      <c r="S22" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -5109,7 +5109,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U22" s="17" t="str">
+      <c r="U22" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -5218,7 +5218,7 @@
         <f t="shared" si="19"/>
         <v>000010</v>
       </c>
-      <c r="S23" s="17" t="str">
+      <c r="S23" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -5226,7 +5226,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U23" s="17" t="str">
+      <c r="U23" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -5265,7 +5265,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B24" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5335,7 +5335,7 @@
         <f t="shared" si="19"/>
         <v>000011</v>
       </c>
-      <c r="S24" s="17" t="str">
+      <c r="S24" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -5343,7 +5343,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U24" s="17" t="str">
+      <c r="U24" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -5452,7 +5452,7 @@
         <f t="shared" si="19"/>
         <v>011001</v>
       </c>
-      <c r="S25" s="17" t="str">
+      <c r="S25" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -5460,7 +5460,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U25" s="17" t="str">
+      <c r="U25" s="25" t="str">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
@@ -5499,7 +5499,7 @@
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B26" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5569,7 +5569,7 @@
         <f t="shared" si="19"/>
         <v>000110</v>
       </c>
-      <c r="S26" s="17" t="str">
+      <c r="S26" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -5577,7 +5577,7 @@
         <f t="shared" si="21"/>
         <v>01010</v>
       </c>
-      <c r="U26" s="17" t="str">
+      <c r="U26" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -5686,7 +5686,7 @@
         <f t="shared" si="19"/>
         <v>011001</v>
       </c>
-      <c r="S27" s="17" t="str">
+      <c r="S27" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -5694,7 +5694,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U27" s="17" t="str">
+      <c r="U27" s="25" t="str">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
@@ -5733,7 +5733,7 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B28" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5803,7 +5803,7 @@
         <f t="shared" si="19"/>
         <v>000110</v>
       </c>
-      <c r="S28" s="17" t="str">
+      <c r="S28" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -5811,7 +5811,7 @@
         <f t="shared" si="21"/>
         <v>10101</v>
       </c>
-      <c r="U28" s="17" t="str">
+      <c r="U28" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -5920,7 +5920,7 @@
         <f t="shared" si="19"/>
         <v>011001</v>
       </c>
-      <c r="S29" s="17" t="str">
+      <c r="S29" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -5928,7 +5928,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U29" s="17" t="str">
+      <c r="U29" s="25" t="str">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
@@ -6037,7 +6037,7 @@
         <f t="shared" si="19"/>
         <v>000010</v>
       </c>
-      <c r="S30" s="17" t="str">
+      <c r="S30" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -6045,7 +6045,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U30" s="17" t="str">
+      <c r="U30" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -6154,7 +6154,7 @@
         <f t="shared" si="19"/>
         <v>000011</v>
       </c>
-      <c r="S31" s="17" t="str">
+      <c r="S31" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -6162,7 +6162,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U31" s="17" t="str">
+      <c r="U31" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -6201,7 +6201,7 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B32" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6271,7 +6271,7 @@
         <f t="shared" si="19"/>
         <v>000111</v>
       </c>
-      <c r="S32" s="17" t="str">
+      <c r="S32" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -6279,7 +6279,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U32" s="17" t="str">
+      <c r="U32" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -6388,7 +6388,7 @@
         <f t="shared" si="19"/>
         <v>000010</v>
       </c>
-      <c r="S33" s="17" t="str">
+      <c r="S33" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -6396,7 +6396,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U33" s="17" t="str">
+      <c r="U33" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -6505,7 +6505,7 @@
         <f t="shared" si="19"/>
         <v>000011</v>
       </c>
-      <c r="S34" s="17" t="str">
+      <c r="S34" s="25" t="str">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
@@ -6513,7 +6513,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U34" s="17" t="str">
+      <c r="U34" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -6622,7 +6622,7 @@
         <f t="shared" si="19"/>
         <v>000010</v>
       </c>
-      <c r="S35" s="17" t="str">
+      <c r="S35" s="25" t="str">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
@@ -6630,7 +6630,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U35" s="17" t="str">
+      <c r="U35" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -6739,7 +6739,7 @@
         <f t="shared" si="19"/>
         <v>000011</v>
       </c>
-      <c r="S36" s="17" t="str">
+      <c r="S36" s="25" t="str">
         <f t="shared" si="20"/>
         <v>10</v>
       </c>
@@ -6747,7 +6747,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U36" s="17" t="str">
+      <c r="U36" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -6856,7 +6856,7 @@
         <f t="shared" si="19"/>
         <v>000011</v>
       </c>
-      <c r="S37" s="17" t="str">
+      <c r="S37" s="25" t="str">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -6864,7 +6864,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U37" s="17" t="str">
+      <c r="U37" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -6973,7 +6973,7 @@
         <f t="shared" si="19"/>
         <v>000011</v>
       </c>
-      <c r="S38" s="17" t="str">
+      <c r="S38" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -6981,7 +6981,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U38" s="17" t="str">
+      <c r="U38" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -7090,7 +7090,7 @@
         <f t="shared" si="19"/>
         <v>000010</v>
       </c>
-      <c r="S39" s="17" t="str">
+      <c r="S39" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -7098,7 +7098,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U39" s="17" t="str">
+      <c r="U39" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -7207,7 +7207,7 @@
         <f t="shared" si="19"/>
         <v>000010</v>
       </c>
-      <c r="S40" s="17" t="str">
+      <c r="S40" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -7215,7 +7215,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U40" s="17" t="str">
+      <c r="U40" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -7324,7 +7324,7 @@
         <f t="shared" si="19"/>
         <v>000001</v>
       </c>
-      <c r="S41" s="17" t="str">
+      <c r="S41" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -7332,7 +7332,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U41" s="17" t="str">
+      <c r="U41" s="25" t="str">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
@@ -7441,7 +7441,7 @@
         <f t="shared" si="19"/>
         <v>000110</v>
       </c>
-      <c r="S42" s="17" t="str">
+      <c r="S42" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -7449,7 +7449,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U42" s="17" t="str">
+      <c r="U42" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -7558,7 +7558,7 @@
         <f t="shared" si="19"/>
         <v>000010</v>
       </c>
-      <c r="S43" s="17" t="str">
+      <c r="S43" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -7566,7 +7566,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U43" s="17" t="str">
+      <c r="U43" s="25" t="str">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
@@ -7675,7 +7675,7 @@
         <f t="shared" si="19"/>
         <v>110001</v>
       </c>
-      <c r="S44" s="17" t="str">
+      <c r="S44" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -7683,7 +7683,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U44" s="17" t="str">
+      <c r="U44" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -7792,7 +7792,7 @@
         <f t="shared" si="19"/>
         <v>000101</v>
       </c>
-      <c r="S45" s="17" t="str">
+      <c r="S45" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -7800,7 +7800,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U45" s="17" t="str">
+      <c r="U45" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -7909,7 +7909,7 @@
         <f t="shared" si="19"/>
         <v>001000</v>
       </c>
-      <c r="S46" s="17" t="str">
+      <c r="S46" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -7917,7 +7917,7 @@
         <f t="shared" si="21"/>
         <v>10</v>
       </c>
-      <c r="U46" s="17" t="str">
+      <c r="U46" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -8026,7 +8026,7 @@
         <f t="shared" si="19"/>
         <v>000010</v>
       </c>
-      <c r="S47" s="17" t="str">
+      <c r="S47" s="25" t="str">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
@@ -8034,7 +8034,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U47" s="17" t="str">
+      <c r="U47" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -8143,7 +8143,7 @@
         <f t="shared" si="19"/>
         <v>010000</v>
       </c>
-      <c r="S48" s="17" t="str">
+      <c r="S48" s="25" t="str">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -8151,7 +8151,7 @@
         <f t="shared" si="21"/>
         <v>10</v>
       </c>
-      <c r="U48" s="17" t="str">
+      <c r="U48" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -8260,7 +8260,7 @@
         <f t="shared" si="19"/>
         <v>000010</v>
       </c>
-      <c r="S49" s="17" t="str">
+      <c r="S49" s="25" t="str">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
@@ -8268,7 +8268,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U49" s="17" t="str">
+      <c r="U49" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -8377,7 +8377,7 @@
         <f t="shared" si="19"/>
         <v>000001</v>
       </c>
-      <c r="S50" s="17" t="str">
+      <c r="S50" s="25" t="str">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -8385,7 +8385,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U50" s="17" t="str">
+      <c r="U50" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -8494,7 +8494,7 @@
         <f t="shared" si="19"/>
         <v>000001</v>
       </c>
-      <c r="S51" s="17" t="str">
+      <c r="S51" s="25" t="str">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
@@ -8502,7 +8502,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U51" s="17" t="str">
+      <c r="U51" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -8611,7 +8611,7 @@
         <f t="shared" si="19"/>
         <v>000010</v>
       </c>
-      <c r="S52" s="17" t="str">
+      <c r="S52" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -8619,7 +8619,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U52" s="17" t="str">
+      <c r="U52" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -8728,7 +8728,7 @@
         <f t="shared" si="19"/>
         <v>000100</v>
       </c>
-      <c r="S53" s="17" t="str">
+      <c r="S53" s="25" t="str">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -8736,7 +8736,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U53" s="17" t="str">
+      <c r="U53" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -8845,7 +8845,7 @@
         <f t="shared" si="19"/>
         <v>110010</v>
       </c>
-      <c r="S54" s="17" t="str">
+      <c r="S54" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -8853,7 +8853,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U54" s="17" t="str">
+      <c r="U54" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -8962,7 +8962,7 @@
         <f t="shared" si="19"/>
         <v>001011</v>
       </c>
-      <c r="S55" s="17" t="str">
+      <c r="S55" s="25" t="str">
         <f t="shared" si="20"/>
         <v>10</v>
       </c>
@@ -8970,7 +8970,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U55" s="17" t="str">
+      <c r="U55" s="25" t="str">
         <f t="shared" si="22"/>
         <v>11</v>
       </c>
@@ -9079,7 +9079,7 @@
         <f t="shared" si="19"/>
         <v>000010</v>
       </c>
-      <c r="S56" s="17" t="str">
+      <c r="S56" s="25" t="str">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -9087,7 +9087,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U56" s="17" t="str">
+      <c r="U56" s="25" t="str">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
@@ -9196,7 +9196,7 @@
         <f t="shared" si="19"/>
         <v>000001</v>
       </c>
-      <c r="S57" s="17" t="str">
+      <c r="S57" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -9204,7 +9204,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U57" s="17" t="str">
+      <c r="U57" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -9313,7 +9313,7 @@
         <f t="shared" si="19"/>
         <v>110010</v>
       </c>
-      <c r="S58" s="17" t="str">
+      <c r="S58" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -9321,7 +9321,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U58" s="17" t="str">
+      <c r="U58" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -9430,7 +9430,7 @@
         <f t="shared" si="19"/>
         <v>000011</v>
       </c>
-      <c r="S59" s="17" t="str">
+      <c r="S59" s="25" t="str">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -9438,7 +9438,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U59" s="17" t="str">
+      <c r="U59" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -9547,7 +9547,7 @@
         <f t="shared" si="19"/>
         <v>001110</v>
       </c>
-      <c r="S60" s="17" t="str">
+      <c r="S60" s="25" t="str">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
@@ -9555,7 +9555,7 @@
         <f t="shared" si="21"/>
         <v>10</v>
       </c>
-      <c r="U60" s="17" t="str">
+      <c r="U60" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -9664,7 +9664,7 @@
         <f t="shared" si="19"/>
         <v>110001</v>
       </c>
-      <c r="S61" s="17" t="str">
+      <c r="S61" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -9672,7 +9672,7 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="U61" s="17" t="str">
+      <c r="U61" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -9781,7 +9781,7 @@
         <f t="shared" si="19"/>
         <v>000101</v>
       </c>
-      <c r="S62" s="17" t="str">
+      <c r="S62" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -9789,7 +9789,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U62" s="17" t="str">
+      <c r="U62" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -9898,7 +9898,7 @@
         <f t="shared" si="19"/>
         <v>001000</v>
       </c>
-      <c r="S63" s="17" t="str">
+      <c r="S63" s="25" t="str">
         <f t="shared" si="20"/>
         <v>11</v>
       </c>
@@ -9906,7 +9906,7 @@
         <f t="shared" si="21"/>
         <v>10</v>
       </c>
-      <c r="U63" s="17" t="str">
+      <c r="U63" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -10015,7 +10015,7 @@
         <f t="shared" si="19"/>
         <v>010000</v>
       </c>
-      <c r="S64" s="17" t="str">
+      <c r="S64" s="25" t="str">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -10023,7 +10023,7 @@
         <f t="shared" si="21"/>
         <v>10</v>
       </c>
-      <c r="U64" s="17" t="str">
+      <c r="U64" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -10132,7 +10132,7 @@
         <f t="shared" si="19"/>
         <v>000010</v>
       </c>
-      <c r="S65" s="17" t="str">
+      <c r="S65" s="25" t="str">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
@@ -10140,7 +10140,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U65" s="17" t="str">
+      <c r="U65" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -10249,7 +10249,7 @@
         <f t="shared" si="19"/>
         <v>000001</v>
       </c>
-      <c r="S66" s="17" t="str">
+      <c r="S66" s="25" t="str">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -10257,7 +10257,7 @@
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="U66" s="17" t="str">
+      <c r="U66" s="25" t="str">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -10366,16 +10366,16 @@
         <f t="shared" ref="R67:R130" si="42">M67</f>
         <v>000010</v>
       </c>
-      <c r="S67" s="17" t="str">
-        <f t="shared" ref="S67:S130" si="43">DEC2BIN(I67)</f>
+      <c r="S67" s="25" t="str">
+        <f t="shared" ref="S67:S130" si="43">IF(ISNUMBER(SEARCH("binary", I67)),MID(I67, 8, 5),DEC2BIN(I67))</f>
         <v>11</v>
       </c>
       <c r="T67" s="25" t="str">
         <f t="shared" ref="T67:T130" si="44">IF(ISNUMBER(SEARCH("binary", J67)),MID(J67, 8, 5),DEC2BIN(J67))</f>
         <v>1</v>
       </c>
-      <c r="U67" s="17" t="str">
-        <f t="shared" ref="U67:U130" si="45">DEC2BIN(K67)</f>
+      <c r="U67" s="25" t="str">
+        <f t="shared" ref="U67:U130" si="45">IF(ISNUMBER(SEARCH("binary", K67)),MID(K67, 8, 5),DEC2BIN(K67))</f>
         <v>0</v>
       </c>
       <c r="V67" s="25" t="str">
@@ -10483,7 +10483,7 @@
         <f t="shared" si="42"/>
         <v>000100</v>
       </c>
-      <c r="S68" s="17" t="str">
+      <c r="S68" s="25" t="str">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -10491,7 +10491,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U68" s="17" t="str">
+      <c r="U68" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -10600,7 +10600,7 @@
         <f t="shared" si="42"/>
         <v>110010</v>
       </c>
-      <c r="S69" s="17" t="str">
+      <c r="S69" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -10608,7 +10608,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U69" s="17" t="str">
+      <c r="U69" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -10717,7 +10717,7 @@
         <f t="shared" si="42"/>
         <v>001011</v>
       </c>
-      <c r="S70" s="17" t="str">
+      <c r="S70" s="25" t="str">
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
@@ -10725,7 +10725,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="U70" s="17" t="str">
+      <c r="U70" s="25" t="str">
         <f t="shared" si="45"/>
         <v>10100</v>
       </c>
@@ -10834,7 +10834,7 @@
         <f t="shared" si="42"/>
         <v>000010</v>
       </c>
-      <c r="S71" s="17" t="str">
+      <c r="S71" s="25" t="str">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -10842,7 +10842,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U71" s="17" t="str">
+      <c r="U71" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -10951,7 +10951,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S72" s="17" t="str">
+      <c r="S72" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -10959,7 +10959,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U72" s="17" t="str">
+      <c r="U72" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -11068,7 +11068,7 @@
         <f t="shared" si="42"/>
         <v>110010</v>
       </c>
-      <c r="S73" s="17" t="str">
+      <c r="S73" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -11076,7 +11076,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U73" s="17" t="str">
+      <c r="U73" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -11185,7 +11185,7 @@
         <f t="shared" si="42"/>
         <v>000011</v>
       </c>
-      <c r="S74" s="17" t="str">
+      <c r="S74" s="25" t="str">
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
@@ -11193,7 +11193,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="U74" s="17" t="str">
+      <c r="U74" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -11302,7 +11302,7 @@
         <f t="shared" si="42"/>
         <v>000011</v>
       </c>
-      <c r="S75" s="17" t="str">
+      <c r="S75" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -11310,7 +11310,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U75" s="17" t="str">
+      <c r="U75" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -11349,7 +11349,7 @@
     </row>
     <row r="76" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B76" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11419,7 +11419,7 @@
         <f t="shared" si="42"/>
         <v>000111</v>
       </c>
-      <c r="S76" s="17" t="str">
+      <c r="S76" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -11427,7 +11427,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U76" s="17" t="str">
+      <c r="U76" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -11536,7 +11536,7 @@
         <f t="shared" si="42"/>
         <v>000010</v>
       </c>
-      <c r="S77" s="17" t="str">
+      <c r="S77" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -11544,7 +11544,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U77" s="17" t="str">
+      <c r="U77" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -11653,7 +11653,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S78" s="17" t="str">
+      <c r="S78" s="25" t="str">
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
@@ -11661,7 +11661,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U78" s="17" t="str">
+      <c r="U78" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -11770,7 +11770,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S79" s="17" t="str">
+      <c r="S79" s="25" t="str">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -11778,7 +11778,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U79" s="17" t="str">
+      <c r="U79" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -11887,7 +11887,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S80" s="17" t="str">
+      <c r="S80" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -11895,7 +11895,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U80" s="17" t="str">
+      <c r="U80" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -12004,7 +12004,7 @@
         <f t="shared" si="42"/>
         <v>000110</v>
       </c>
-      <c r="S81" s="17" t="str">
+      <c r="S81" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -12012,7 +12012,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U81" s="17" t="str">
+      <c r="U81" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -12121,7 +12121,7 @@
         <f t="shared" si="42"/>
         <v>000010</v>
       </c>
-      <c r="S82" s="17" t="str">
+      <c r="S82" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -12129,7 +12129,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U82" s="17" t="str">
+      <c r="U82" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -12238,7 +12238,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S83" s="17" t="str">
+      <c r="S83" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -12246,7 +12246,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U83" s="17" t="str">
+      <c r="U83" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -12355,7 +12355,7 @@
         <f t="shared" si="42"/>
         <v>000101</v>
       </c>
-      <c r="S84" s="17" t="str">
+      <c r="S84" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -12363,7 +12363,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U84" s="17" t="str">
+      <c r="U84" s="25" t="str">
         <f t="shared" si="45"/>
         <v>1</v>
       </c>
@@ -12472,7 +12472,7 @@
         <f t="shared" si="42"/>
         <v>001010</v>
       </c>
-      <c r="S85" s="17" t="str">
+      <c r="S85" s="25" t="str">
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
@@ -12480,7 +12480,7 @@
         <f t="shared" si="44"/>
         <v>11</v>
       </c>
-      <c r="U85" s="17" t="str">
+      <c r="U85" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -12589,7 +12589,7 @@
         <f t="shared" si="42"/>
         <v>001011</v>
       </c>
-      <c r="S86" s="17" t="str">
+      <c r="S86" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -12597,7 +12597,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="U86" s="17" t="str">
+      <c r="U86" s="25" t="str">
         <f t="shared" si="45"/>
         <v>1001</v>
       </c>
@@ -12706,7 +12706,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S87" s="17" t="str">
+      <c r="S87" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -12714,7 +12714,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U87" s="17" t="str">
+      <c r="U87" s="25" t="str">
         <f t="shared" si="45"/>
         <v>1</v>
       </c>
@@ -12823,7 +12823,7 @@
         <f t="shared" si="42"/>
         <v>000101</v>
       </c>
-      <c r="S88" s="17" t="str">
+      <c r="S88" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -12831,7 +12831,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U88" s="17" t="str">
+      <c r="U88" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -12940,7 +12940,7 @@
         <f t="shared" si="42"/>
         <v>000101</v>
       </c>
-      <c r="S89" s="17" t="str">
+      <c r="S89" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -12948,7 +12948,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U89" s="17" t="str">
+      <c r="U89" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -13057,7 +13057,7 @@
         <f t="shared" si="42"/>
         <v>001010</v>
       </c>
-      <c r="S90" s="17" t="str">
+      <c r="S90" s="25" t="str">
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
@@ -13065,7 +13065,7 @@
         <f t="shared" si="44"/>
         <v>11</v>
       </c>
-      <c r="U90" s="17" t="str">
+      <c r="U90" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -13174,7 +13174,7 @@
         <f t="shared" si="42"/>
         <v>001011</v>
       </c>
-      <c r="S91" s="17" t="str">
+      <c r="S91" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -13182,7 +13182,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="U91" s="17" t="str">
+      <c r="U91" s="25" t="str">
         <f t="shared" si="45"/>
         <v>1110</v>
       </c>
@@ -13291,7 +13291,7 @@
         <f t="shared" si="42"/>
         <v>000010</v>
       </c>
-      <c r="S92" s="17" t="str">
+      <c r="S92" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -13299,7 +13299,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U92" s="17" t="str">
+      <c r="U92" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -13408,7 +13408,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S93" s="17" t="str">
+      <c r="S93" s="25" t="str">
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
@@ -13416,7 +13416,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U93" s="17" t="str">
+      <c r="U93" s="25" t="str">
         <f t="shared" si="45"/>
         <v>1</v>
       </c>
@@ -13525,7 +13525,7 @@
         <f t="shared" si="42"/>
         <v>001110</v>
       </c>
-      <c r="S94" s="17" t="str">
+      <c r="S94" s="25" t="str">
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
@@ -13533,7 +13533,7 @@
         <f t="shared" si="44"/>
         <v>11</v>
       </c>
-      <c r="U94" s="17" t="str">
+      <c r="U94" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -13642,7 +13642,7 @@
         <f t="shared" si="42"/>
         <v>000011</v>
       </c>
-      <c r="S95" s="17" t="str">
+      <c r="S95" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -13650,7 +13650,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="U95" s="17" t="str">
+      <c r="U95" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -13689,7 +13689,7 @@
     </row>
     <row r="96" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A96" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B96" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13759,7 +13759,7 @@
         <f t="shared" si="42"/>
         <v>000110</v>
       </c>
-      <c r="S96" s="17" t="str">
+      <c r="S96" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -13767,7 +13767,7 @@
         <f t="shared" si="44"/>
         <v>11110</v>
       </c>
-      <c r="U96" s="17" t="str">
+      <c r="U96" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -13806,7 +13806,7 @@
     </row>
     <row r="97" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B97" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13876,7 +13876,7 @@
         <f t="shared" si="42"/>
         <v>000110</v>
       </c>
-      <c r="S97" s="17" t="str">
+      <c r="S97" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -13884,7 +13884,7 @@
         <f t="shared" si="44"/>
         <v>1010</v>
       </c>
-      <c r="U97" s="17" t="str">
+      <c r="U97" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -13993,7 +13993,7 @@
         <f t="shared" si="42"/>
         <v>000010</v>
       </c>
-      <c r="S98" s="17" t="str">
+      <c r="S98" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -14001,7 +14001,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="U98" s="17" t="str">
+      <c r="U98" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -14110,7 +14110,7 @@
         <f t="shared" si="42"/>
         <v>100001</v>
       </c>
-      <c r="S99" s="17" t="str">
+      <c r="S99" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -14118,7 +14118,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="U99" s="17" t="str">
+      <c r="U99" s="25" t="str">
         <f t="shared" si="45"/>
         <v>11101</v>
       </c>
@@ -14227,7 +14227,7 @@
         <f t="shared" si="42"/>
         <v>000010</v>
       </c>
-      <c r="S100" s="17" t="str">
+      <c r="S100" s="25" t="str">
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
@@ -14235,7 +14235,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U100" s="17" t="str">
+      <c r="U100" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -14344,7 +14344,7 @@
         <f t="shared" si="42"/>
         <v>000011</v>
       </c>
-      <c r="S101" s="17" t="str">
+      <c r="S101" s="25" t="str">
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
@@ -14352,7 +14352,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="U101" s="17" t="str">
+      <c r="U101" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -14461,7 +14461,7 @@
         <f t="shared" si="42"/>
         <v>000011</v>
       </c>
-      <c r="S102" s="17" t="str">
+      <c r="S102" s="25" t="str">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -14469,7 +14469,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="U102" s="17" t="str">
+      <c r="U102" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -14578,7 +14578,7 @@
         <f t="shared" si="42"/>
         <v>010000</v>
       </c>
-      <c r="S103" s="17" t="str">
+      <c r="S103" s="25" t="str">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -14586,7 +14586,7 @@
         <f t="shared" si="44"/>
         <v>10</v>
       </c>
-      <c r="U103" s="17" t="str">
+      <c r="U103" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -14695,7 +14695,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S104" s="17" t="str">
+      <c r="S104" s="25" t="str">
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
@@ -14703,7 +14703,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U104" s="17" t="str">
+      <c r="U104" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -14812,7 +14812,7 @@
         <f t="shared" si="42"/>
         <v>000010</v>
       </c>
-      <c r="S105" s="17" t="str">
+      <c r="S105" s="25" t="str">
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
@@ -14820,7 +14820,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U105" s="17" t="str">
+      <c r="U105" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -14929,7 +14929,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S106" s="17" t="str">
+      <c r="S106" s="25" t="str">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -14937,7 +14937,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U106" s="17" t="str">
+      <c r="U106" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -15046,7 +15046,7 @@
         <f t="shared" si="42"/>
         <v>010000</v>
       </c>
-      <c r="S107" s="17" t="str">
+      <c r="S107" s="25" t="str">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -15054,7 +15054,7 @@
         <f t="shared" si="44"/>
         <v>10</v>
       </c>
-      <c r="U107" s="17" t="str">
+      <c r="U107" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -15163,7 +15163,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S108" s="17" t="str">
+      <c r="S108" s="25" t="str">
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
@@ -15171,7 +15171,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U108" s="17" t="str">
+      <c r="U108" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -15280,7 +15280,7 @@
         <f t="shared" si="42"/>
         <v>000010</v>
       </c>
-      <c r="S109" s="17" t="str">
+      <c r="S109" s="25" t="str">
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
@@ -15288,7 +15288,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U109" s="17" t="str">
+      <c r="U109" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -15397,7 +15397,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S110" s="17" t="str">
+      <c r="S110" s="25" t="str">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -15405,7 +15405,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U110" s="17" t="str">
+      <c r="U110" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -15514,7 +15514,7 @@
         <f t="shared" si="42"/>
         <v>010000</v>
       </c>
-      <c r="S111" s="17" t="str">
+      <c r="S111" s="25" t="str">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -15522,7 +15522,7 @@
         <f t="shared" si="44"/>
         <v>10</v>
       </c>
-      <c r="U111" s="17" t="str">
+      <c r="U111" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -15631,7 +15631,7 @@
         <f t="shared" si="42"/>
         <v>000010</v>
       </c>
-      <c r="S112" s="17" t="str">
+      <c r="S112" s="25" t="str">
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
@@ -15639,7 +15639,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U112" s="17" t="str">
+      <c r="U112" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -15748,7 +15748,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S113" s="17" t="str">
+      <c r="S113" s="25" t="str">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -15756,7 +15756,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U113" s="17" t="str">
+      <c r="U113" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -15865,7 +15865,7 @@
         <f t="shared" si="42"/>
         <v>000011</v>
       </c>
-      <c r="S114" s="17" t="str">
+      <c r="S114" s="25" t="str">
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
@@ -15873,7 +15873,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="U114" s="17" t="str">
+      <c r="U114" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -15982,7 +15982,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S115" s="17" t="str">
+      <c r="S115" s="25" t="str">
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
@@ -15990,7 +15990,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U115" s="17" t="str">
+      <c r="U115" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -16099,7 +16099,7 @@
         <f t="shared" si="42"/>
         <v>010001</v>
       </c>
-      <c r="S116" s="17" t="str">
+      <c r="S116" s="25" t="str">
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
@@ -16107,7 +16107,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="U116" s="17" t="str">
+      <c r="U116" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -16216,7 +16216,7 @@
         <f t="shared" si="42"/>
         <v>001000</v>
       </c>
-      <c r="S117" s="17" t="str">
+      <c r="S117" s="25" t="str">
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
@@ -16224,7 +16224,7 @@
         <f t="shared" si="44"/>
         <v>11</v>
       </c>
-      <c r="U117" s="17" t="str">
+      <c r="U117" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -16333,7 +16333,7 @@
         <f t="shared" si="42"/>
         <v>110010</v>
       </c>
-      <c r="S118" s="17" t="str">
+      <c r="S118" s="25" t="str">
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
@@ -16341,7 +16341,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U118" s="17" t="str">
+      <c r="U118" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -16450,7 +16450,7 @@
         <f t="shared" si="42"/>
         <v>000011</v>
       </c>
-      <c r="S119" s="17" t="str">
+      <c r="S119" s="25" t="str">
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
@@ -16458,7 +16458,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="U119" s="17" t="str">
+      <c r="U119" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -16567,7 +16567,7 @@
         <f t="shared" si="42"/>
         <v>000011</v>
       </c>
-      <c r="S120" s="17" t="str">
+      <c r="S120" s="25" t="str">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -16575,7 +16575,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U120" s="17" t="str">
+      <c r="U120" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -16684,7 +16684,7 @@
         <f t="shared" si="42"/>
         <v>000010</v>
       </c>
-      <c r="S121" s="17" t="str">
+      <c r="S121" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -16692,7 +16692,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U121" s="17" t="str">
+      <c r="U121" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -16801,7 +16801,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S122" s="17" t="str">
+      <c r="S122" s="25" t="str">
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
@@ -16809,7 +16809,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U122" s="17" t="str">
+      <c r="U122" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -16918,7 +16918,7 @@
         <f t="shared" si="42"/>
         <v>010001</v>
       </c>
-      <c r="S123" s="17" t="str">
+      <c r="S123" s="25" t="str">
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
@@ -16926,7 +16926,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="U123" s="17" t="str">
+      <c r="U123" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -17035,7 +17035,7 @@
         <f t="shared" si="42"/>
         <v>001000</v>
       </c>
-      <c r="S124" s="17" t="str">
+      <c r="S124" s="25" t="str">
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
@@ -17043,7 +17043,7 @@
         <f t="shared" si="44"/>
         <v>11</v>
       </c>
-      <c r="U124" s="17" t="str">
+      <c r="U124" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -17152,7 +17152,7 @@
         <f t="shared" si="42"/>
         <v>001000</v>
       </c>
-      <c r="S125" s="17" t="str">
+      <c r="S125" s="25" t="str">
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
@@ -17160,7 +17160,7 @@
         <f t="shared" si="44"/>
         <v>11</v>
       </c>
-      <c r="U125" s="17" t="str">
+      <c r="U125" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -17269,7 +17269,7 @@
         <f t="shared" si="42"/>
         <v>110010</v>
       </c>
-      <c r="S126" s="17" t="str">
+      <c r="S126" s="25" t="str">
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
@@ -17277,7 +17277,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U126" s="17" t="str">
+      <c r="U126" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -17386,7 +17386,7 @@
         <f t="shared" si="42"/>
         <v>000011</v>
       </c>
-      <c r="S127" s="17" t="str">
+      <c r="S127" s="25" t="str">
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
@@ -17394,7 +17394,7 @@
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="U127" s="17" t="str">
+      <c r="U127" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -17503,7 +17503,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S128" s="17" t="str">
+      <c r="S128" s="25" t="str">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
@@ -17511,7 +17511,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U128" s="17" t="str">
+      <c r="U128" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -17620,7 +17620,7 @@
         <f t="shared" si="42"/>
         <v>000010</v>
       </c>
-      <c r="S129" s="17" t="str">
+      <c r="S129" s="25" t="str">
         <f t="shared" si="43"/>
         <v>11</v>
       </c>
@@ -17628,7 +17628,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U129" s="17" t="str">
+      <c r="U129" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -17737,7 +17737,7 @@
         <f t="shared" si="42"/>
         <v>000001</v>
       </c>
-      <c r="S130" s="17" t="str">
+      <c r="S130" s="25" t="str">
         <f t="shared" si="43"/>
         <v>10</v>
       </c>
@@ -17745,7 +17745,7 @@
         <f t="shared" si="44"/>
         <v>1</v>
       </c>
-      <c r="U130" s="17" t="str">
+      <c r="U130" s="25" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -17854,16 +17854,16 @@
         <f t="shared" ref="R131:R146" si="65">M131</f>
         <v>010001</v>
       </c>
-      <c r="S131" s="17" t="str">
-        <f t="shared" ref="S131:S146" si="66">DEC2BIN(I131)</f>
+      <c r="S131" s="25" t="str">
+        <f t="shared" ref="S131:S146" si="66">IF(ISNUMBER(SEARCH("binary", I131)),MID(I131, 8, 5),DEC2BIN(I131))</f>
         <v>10</v>
       </c>
       <c r="T131" s="25" t="str">
         <f t="shared" ref="T131:T146" si="67">IF(ISNUMBER(SEARCH("binary", J131)),MID(J131, 8, 5),DEC2BIN(J131))</f>
         <v>0</v>
       </c>
-      <c r="U131" s="17" t="str">
-        <f t="shared" ref="U131:U146" si="68">DEC2BIN(K131)</f>
+      <c r="U131" s="25" t="str">
+        <f t="shared" ref="U131:U146" si="68">IF(ISNUMBER(SEARCH("binary", K131)),MID(K131, 8, 5),DEC2BIN(K131))</f>
         <v>0</v>
       </c>
       <c r="V131" s="25" t="str">
@@ -17971,7 +17971,7 @@
         <f t="shared" si="65"/>
         <v>001000</v>
       </c>
-      <c r="S132" s="17" t="str">
+      <c r="S132" s="25" t="str">
         <f t="shared" si="66"/>
         <v>1</v>
       </c>
@@ -17979,7 +17979,7 @@
         <f t="shared" si="67"/>
         <v>11</v>
       </c>
-      <c r="U132" s="17" t="str">
+      <c r="U132" s="25" t="str">
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
@@ -18088,7 +18088,7 @@
         <f t="shared" si="65"/>
         <v>001000</v>
       </c>
-      <c r="S133" s="17" t="str">
+      <c r="S133" s="25" t="str">
         <f t="shared" si="66"/>
         <v>10</v>
       </c>
@@ -18096,7 +18096,7 @@
         <f t="shared" si="67"/>
         <v>11</v>
       </c>
-      <c r="U133" s="17" t="str">
+      <c r="U133" s="25" t="str">
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
@@ -18205,7 +18205,7 @@
         <f t="shared" si="65"/>
         <v>110010</v>
       </c>
-      <c r="S134" s="17" t="str">
+      <c r="S134" s="25" t="str">
         <f t="shared" si="66"/>
         <v>10</v>
       </c>
@@ -18213,7 +18213,7 @@
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
-      <c r="U134" s="17" t="str">
+      <c r="U134" s="25" t="str">
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
@@ -18322,7 +18322,7 @@
         <f t="shared" si="65"/>
         <v>000011</v>
       </c>
-      <c r="S135" s="17" t="str">
+      <c r="S135" s="25" t="str">
         <f t="shared" si="66"/>
         <v>1</v>
       </c>
@@ -18330,7 +18330,7 @@
         <f t="shared" si="67"/>
         <v>0</v>
       </c>
-      <c r="U135" s="17" t="str">
+      <c r="U135" s="25" t="str">
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
@@ -18439,7 +18439,7 @@
         <f t="shared" si="65"/>
         <v>000011</v>
       </c>
-      <c r="S136" s="17" t="str">
+      <c r="S136" s="25" t="str">
         <f t="shared" si="66"/>
         <v>10</v>
       </c>
@@ -18447,7 +18447,7 @@
         <f t="shared" si="67"/>
         <v>0</v>
       </c>
-      <c r="U136" s="17" t="str">
+      <c r="U136" s="25" t="str">
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
@@ -18556,7 +18556,7 @@
         <f t="shared" si="65"/>
         <v>000010</v>
       </c>
-      <c r="S137" s="17" t="str">
+      <c r="S137" s="25" t="str">
         <f t="shared" si="66"/>
         <v>11</v>
       </c>
@@ -18564,7 +18564,7 @@
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
-      <c r="U137" s="17" t="str">
+      <c r="U137" s="25" t="str">
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
@@ -18673,7 +18673,7 @@
         <f t="shared" si="65"/>
         <v>000001</v>
       </c>
-      <c r="S138" s="17" t="str">
+      <c r="S138" s="25" t="str">
         <f t="shared" si="66"/>
         <v>10</v>
       </c>
@@ -18681,7 +18681,7 @@
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
-      <c r="U138" s="17" t="str">
+      <c r="U138" s="25" t="str">
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
@@ -18790,7 +18790,7 @@
         <f t="shared" si="65"/>
         <v>010001</v>
       </c>
-      <c r="S139" s="17" t="str">
+      <c r="S139" s="25" t="str">
         <f t="shared" si="66"/>
         <v>10</v>
       </c>
@@ -18798,7 +18798,7 @@
         <f t="shared" si="67"/>
         <v>0</v>
       </c>
-      <c r="U139" s="17" t="str">
+      <c r="U139" s="25" t="str">
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
@@ -18907,7 +18907,7 @@
         <f t="shared" si="65"/>
         <v>001000</v>
       </c>
-      <c r="S140" s="17" t="str">
+      <c r="S140" s="25" t="str">
         <f t="shared" si="66"/>
         <v>1</v>
       </c>
@@ -18915,7 +18915,7 @@
         <f t="shared" si="67"/>
         <v>11</v>
       </c>
-      <c r="U140" s="17" t="str">
+      <c r="U140" s="25" t="str">
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
@@ -18954,7 +18954,7 @@
     </row>
     <row r="141" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A141" s="12" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="B141" s="9" t="str">
         <f t="shared" si="54"/>
@@ -18962,7 +18962,7 @@
       </c>
       <c r="C141" s="9">
         <f t="shared" si="55"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D141" s="8">
         <f t="shared" si="56"/>
@@ -18978,11 +18978,11 @@
       </c>
       <c r="G141" s="8">
         <f t="shared" si="59"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H141" s="8">
         <f t="shared" si="60"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I141" s="9" t="str">
         <f t="shared" si="61"/>
@@ -18994,11 +18994,11 @@
       </c>
       <c r="K141" s="9" t="str">
         <f t="shared" si="63"/>
+        <v>0</v>
+      </c>
+      <c r="L141" s="9" t="str">
+        <f t="shared" si="64"/>
         <v>23</v>
-      </c>
-      <c r="L141" s="9">
-        <f t="shared" si="64"/>
-        <v>0</v>
       </c>
       <c r="M141" s="22" t="str">
         <f>VLOOKUP($B141,'Conversion to binary Key'!$D:$I,2,0)</f>
@@ -19024,7 +19024,7 @@
         <f t="shared" si="65"/>
         <v>001000</v>
       </c>
-      <c r="S141" s="17" t="str">
+      <c r="S141" s="25" t="str">
         <f t="shared" si="66"/>
         <v>10</v>
       </c>
@@ -19032,12 +19032,13 @@
         <f t="shared" si="67"/>
         <v>11</v>
       </c>
-      <c r="U141" s="17" t="s">
-        <v>102</v>
+      <c r="U141" s="25" t="str">
+        <f t="shared" si="68"/>
+        <v>0</v>
       </c>
       <c r="V141" s="25" t="str">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>10111</v>
       </c>
       <c r="W141" s="15" t="str">
         <f t="shared" si="70"/>
@@ -19057,11 +19058,11 @@
       </c>
       <c r="AA141" s="10" t="str">
         <f t="shared" si="74"/>
-        <v>00000</v>
+        <v>10111</v>
       </c>
       <c r="AB141" s="11" t="str">
         <f t="shared" si="75"/>
-        <v>0010001011000000</v>
+        <v>0010001011010111</v>
       </c>
       <c r="AC141" s="10">
         <f t="shared" si="53"/>
@@ -19140,7 +19141,7 @@
         <f t="shared" si="65"/>
         <v>110010</v>
       </c>
-      <c r="S142" s="17" t="str">
+      <c r="S142" s="25" t="str">
         <f t="shared" si="66"/>
         <v>10</v>
       </c>
@@ -19148,7 +19149,7 @@
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
-      <c r="U142" s="17" t="str">
+      <c r="U142" s="25" t="str">
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
@@ -19257,7 +19258,7 @@
         <f t="shared" si="65"/>
         <v>110010</v>
       </c>
-      <c r="S143" s="17" t="str">
+      <c r="S143" s="25" t="str">
         <f t="shared" si="66"/>
         <v>11</v>
       </c>
@@ -19265,7 +19266,7 @@
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
-      <c r="U143" s="17" t="str">
+      <c r="U143" s="25" t="str">
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
@@ -19374,7 +19375,7 @@
         <f t="shared" si="65"/>
         <v>000001</v>
       </c>
-      <c r="S144" s="17" t="str">
+      <c r="S144" s="25" t="str">
         <f t="shared" si="66"/>
         <v>11</v>
       </c>
@@ -19382,7 +19383,7 @@
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
-      <c r="U144" s="17" t="str">
+      <c r="U144" s="25" t="str">
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
@@ -19491,7 +19492,7 @@
         <f t="shared" si="65"/>
         <v>110010</v>
       </c>
-      <c r="S145" s="17" t="str">
+      <c r="S145" s="25" t="str">
         <f t="shared" si="66"/>
         <v>11</v>
       </c>
@@ -19499,7 +19500,7 @@
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
-      <c r="U145" s="17" t="str">
+      <c r="U145" s="25" t="str">
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
@@ -19608,7 +19609,7 @@
         <f t="shared" si="65"/>
         <v>000000</v>
       </c>
-      <c r="S146" s="17" t="str">
+      <c r="S146" s="25" t="str">
         <f t="shared" si="66"/>
         <v>0</v>
       </c>
@@ -19616,7 +19617,7 @@
         <f t="shared" si="67"/>
         <v>0</v>
       </c>
-      <c r="U146" s="17" t="str">
+      <c r="U146" s="25" t="str">
         <f t="shared" si="68"/>
         <v>0</v>
       </c>
@@ -19658,18 +19659,30 @@
       <c r="N147"/>
       <c r="O147"/>
       <c r="P147"/>
+      <c r="U147" s="17" t="str">
+        <f t="shared" ref="U146:U149" si="76">DEC2BIN(K147)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="148" spans="1:29" x14ac:dyDescent="0.3">
       <c r="M148"/>
       <c r="N148"/>
       <c r="O148"/>
       <c r="P148"/>
+      <c r="U148" s="17" t="str">
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="149" spans="1:29" x14ac:dyDescent="0.3">
       <c r="M149"/>
       <c r="N149"/>
       <c r="O149"/>
       <c r="P149"/>
+      <c r="U149" s="17" t="str">
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="150" spans="1:29" x14ac:dyDescent="0.3">
       <c r="M150"/>
@@ -20274,9 +20287,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="T2:T146" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Program 1 fixes (ongoing)
</commit_message>
<xml_diff>
--- a/Convert to Binary_v3 - Program 1.xlsx
+++ b/Convert to Binary_v3 - Program 1.xlsx
@@ -637,9 +637,6 @@
     <t>Set R0 contents back to 0</t>
   </si>
   <si>
-    <t>SOB 1,2,0,0(aifls)</t>
-  </si>
-  <si>
     <t>Subtract 1 from R1 and if &gt; 0, branch back to ARRAY INPUT FOR LOOP START</t>
   </si>
   <si>
@@ -992,6 +989,9 @@
   </si>
   <si>
     <t>JZ 2,3,0,26(g1p)</t>
+  </si>
+  <si>
+    <t>SOB 1,2,0,1(aifls)</t>
   </si>
 </sst>
 </file>
@@ -1212,7 +1212,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1525,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1578,12 +1585,12 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1601,15 +1608,15 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1643,7 +1650,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D17" t="s">
         <v>152</v>
@@ -1656,7 +1663,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D19" t="s">
         <v>153</v>
@@ -1669,7 +1676,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F21" t="s">
         <v>155</v>
@@ -1685,10 +1692,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1701,7 +1708,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1711,7 +1718,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1740,7 +1747,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1846,18 +1853,18 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>294</v>
+      </c>
+      <c r="D45" t="s">
         <v>295</v>
-      </c>
-      <c r="D45" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>289</v>
+      </c>
+      <c r="D46" t="s">
         <v>290</v>
-      </c>
-      <c r="D46" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -1865,7 +1872,7 @@
         <v>168</v>
       </c>
       <c r="E47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -1939,7 +1946,7 @@
         <v>200</v>
       </c>
       <c r="E57" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -1957,10 +1964,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>320</v>
+      </c>
+      <c r="D60" t="s">
         <v>202</v>
-      </c>
-      <c r="D60" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -1968,7 +1975,7 @@
         <v>180</v>
       </c>
       <c r="G61" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -1976,23 +1983,23 @@
         <v>182</v>
       </c>
       <c r="E62" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D63" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E64" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -2000,7 +2007,7 @@
         <v>184</v>
       </c>
       <c r="G65" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2008,7 +2015,7 @@
         <v>186</v>
       </c>
       <c r="E66" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -2021,7 +2028,7 @@
         <v>191</v>
       </c>
       <c r="E68" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -2039,26 +2046,26 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>306</v>
+      </c>
+      <c r="G72" t="s">
         <v>307</v>
-      </c>
-      <c r="G72" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>208</v>
+      </c>
+      <c r="E73" t="s">
         <v>209</v>
-      </c>
-      <c r="E73" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -2066,7 +2073,7 @@
         <v>200</v>
       </c>
       <c r="E74" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -2079,7 +2086,7 @@
         <v>166</v>
       </c>
       <c r="E76" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -2087,12 +2094,12 @@
         <v>162</v>
       </c>
       <c r="E77" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -2102,26 +2109,26 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>213</v>
+      </c>
+      <c r="E80" t="s">
         <v>214</v>
-      </c>
-      <c r="E80" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>215</v>
+      </c>
+      <c r="E81" t="s">
         <v>216</v>
-      </c>
-      <c r="E81" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
+        <v>217</v>
+      </c>
+      <c r="E82" t="s">
         <v>218</v>
-      </c>
-      <c r="E82" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -2142,34 +2149,34 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>219</v>
+      </c>
+      <c r="E85" t="s">
         <v>220</v>
-      </c>
-      <c r="E85" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
+        <v>221</v>
+      </c>
+      <c r="E86" t="s">
         <v>222</v>
-      </c>
-      <c r="E86" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D87" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E88" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -2177,84 +2184,84 @@
         <v>176</v>
       </c>
       <c r="E89" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
+        <v>226</v>
+      </c>
+      <c r="E90" t="s">
         <v>227</v>
-      </c>
-      <c r="E90" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
+        <v>228</v>
+      </c>
+      <c r="E91" t="s">
         <v>229</v>
-      </c>
-      <c r="E91" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D92" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E93" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E94" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
+        <v>233</v>
+      </c>
+      <c r="E95" t="s">
         <v>234</v>
-      </c>
-      <c r="E95" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D96" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
+        <v>236</v>
+      </c>
+      <c r="E97" t="s">
         <v>237</v>
-      </c>
-      <c r="E97" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F98" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -2262,7 +2269,7 @@
         <v>144</v>
       </c>
       <c r="E100" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -2272,10 +2279,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>240</v>
+      </c>
+      <c r="E102" t="s">
         <v>241</v>
-      </c>
-      <c r="E102" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -2283,7 +2290,7 @@
         <v>3</v>
       </c>
       <c r="E103" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -2291,7 +2298,7 @@
         <v>9</v>
       </c>
       <c r="E104" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
@@ -2299,15 +2306,15 @@
         <v>184</v>
       </c>
       <c r="G105" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E106" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
@@ -2315,7 +2322,7 @@
         <v>186</v>
       </c>
       <c r="E107" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
@@ -2328,15 +2335,15 @@
         <v>184</v>
       </c>
       <c r="G109" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E110" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
@@ -2344,7 +2351,7 @@
         <v>186</v>
       </c>
       <c r="E111" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
@@ -2357,7 +2364,7 @@
         <v>184</v>
       </c>
       <c r="G113" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
@@ -2365,7 +2372,7 @@
         <v>186</v>
       </c>
       <c r="E114" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
@@ -2378,15 +2385,15 @@
         <v>10</v>
       </c>
       <c r="F116" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
+        <v>251</v>
+      </c>
+      <c r="E117" t="s">
         <v>252</v>
-      </c>
-      <c r="E117" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
@@ -2394,23 +2401,23 @@
         <v>11</v>
       </c>
       <c r="G118" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D119" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
+        <v>255</v>
+      </c>
+      <c r="G120" t="s">
         <v>256</v>
-      </c>
-      <c r="G120" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
@@ -2418,15 +2425,15 @@
         <v>12</v>
       </c>
       <c r="F121" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
+        <v>258</v>
+      </c>
+      <c r="E122" t="s">
         <v>259</v>
-      </c>
-      <c r="E122" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
@@ -2434,12 +2441,12 @@
         <v>191</v>
       </c>
       <c r="E123" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
@@ -2447,31 +2454,31 @@
         <v>11</v>
       </c>
       <c r="G125" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D126" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D127" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G128" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -2479,15 +2486,15 @@
         <v>12</v>
       </c>
       <c r="F129" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
+        <v>266</v>
+      </c>
+      <c r="E130" t="s">
         <v>267</v>
-      </c>
-      <c r="E130" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
@@ -2495,12 +2502,12 @@
         <v>191</v>
       </c>
       <c r="E131" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
@@ -2508,31 +2515,31 @@
         <v>11</v>
       </c>
       <c r="G133" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D134" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D135" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G136" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
@@ -2540,7 +2547,7 @@
         <v>12</v>
       </c>
       <c r="F137" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
@@ -2548,7 +2555,7 @@
         <v>3</v>
       </c>
       <c r="E138" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
@@ -2556,12 +2563,12 @@
         <v>191</v>
       </c>
       <c r="E139" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
@@ -2569,31 +2576,31 @@
         <v>11</v>
       </c>
       <c r="G141" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D142" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D143" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G144" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
@@ -2601,7 +2608,7 @@
         <v>194</v>
       </c>
       <c r="G145" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
@@ -2609,7 +2616,7 @@
         <v>200</v>
       </c>
       <c r="E146" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
@@ -2622,7 +2629,7 @@
         <v>13</v>
       </c>
       <c r="H148" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -2635,10 +2642,10 @@
   <dimension ref="A1:AD248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O119" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="AJ141" sqref="AJ141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3448,7 +3455,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B8" s="9" t="str">
         <f t="shared" si="8"/>
@@ -3565,7 +3572,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B9" s="9" t="str">
         <f t="shared" si="8"/>
@@ -3916,7 +3923,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B12" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4033,7 +4040,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B13" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4618,7 +4625,7 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B18" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4852,7 +4859,7 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B20" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5086,7 +5093,7 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B22" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5320,7 +5327,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B24" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5554,7 +5561,7 @@
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B26" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5788,7 +5795,7 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B28" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6256,7 +6263,7 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B32" s="9" t="str">
         <f t="shared" si="8"/>
@@ -7894,7 +7901,7 @@
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B46" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8011,7 +8018,7 @@
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B47" s="9" t="str">
         <f t="shared" si="8"/>
@@ -9649,7 +9656,7 @@
     </row>
     <row r="61" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A61" s="12" t="s">
-        <v>202</v>
+        <v>320</v>
       </c>
       <c r="B61" s="9" t="str">
         <f t="shared" si="8"/>
@@ -9693,7 +9700,7 @@
       </c>
       <c r="L61" s="9" t="str">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M61" s="22" t="str">
         <f>VLOOKUP($B61,'Conversion to binary Key'!$D:$I,2,0)</f>
@@ -9733,7 +9740,7 @@
       </c>
       <c r="V61" s="25" t="str">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W61" s="15" t="str">
         <f t="shared" si="24"/>
@@ -9753,11 +9760,11 @@
       </c>
       <c r="AA61" s="10" t="str">
         <f t="shared" si="28"/>
-        <v>00000</v>
+        <v>00001</v>
       </c>
       <c r="AB61" s="11" t="str">
         <f t="shared" si="29"/>
-        <v>0011100110000000</v>
+        <v>0011100110000001</v>
       </c>
       <c r="AC61" s="10">
         <f t="shared" si="7"/>
@@ -10000,7 +10007,7 @@
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B64" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10117,7 +10124,7 @@
     </row>
     <row r="65" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B65" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10936,7 +10943,7 @@
     </row>
     <row r="72" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A72" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B72" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11053,7 +11060,7 @@
     </row>
     <row r="73" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B73" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11170,7 +11177,7 @@
     </row>
     <row r="74" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A74" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B74" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11755,7 +11762,7 @@
     </row>
     <row r="79" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A79" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B79" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11989,7 +11996,7 @@
     </row>
     <row r="81" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A81" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B81" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12106,7 +12113,7 @@
     </row>
     <row r="82" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A82" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B82" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12223,7 +12230,7 @@
     </row>
     <row r="83" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A83" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B83" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12574,7 +12581,7 @@
     </row>
     <row r="86" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A86" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B86" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12691,7 +12698,7 @@
     </row>
     <row r="87" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A87" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B87" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12808,7 +12815,7 @@
     </row>
     <row r="88" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A88" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B88" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12925,7 +12932,7 @@
     </row>
     <row r="89" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B89" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13159,7 +13166,7 @@
     </row>
     <row r="91" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A91" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B91" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13276,7 +13283,7 @@
     </row>
     <row r="92" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A92" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B92" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13393,7 +13400,7 @@
     </row>
     <row r="93" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A93" s="12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B93" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13510,7 +13517,7 @@
     </row>
     <row r="94" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A94" s="12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B94" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13627,7 +13634,7 @@
     </row>
     <row r="95" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A95" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B95" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13744,7 +13751,7 @@
     </row>
     <row r="96" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A96" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B96" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13861,7 +13868,7 @@
     </row>
     <row r="97" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B97" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13978,7 +13985,7 @@
     </row>
     <row r="98" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A98" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B98" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14095,7 +14102,7 @@
     </row>
     <row r="99" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A99" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B99" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14212,7 +14219,7 @@
     </row>
     <row r="100" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B100" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14563,7 +14570,7 @@
     </row>
     <row r="103" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B103" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15031,7 +15038,7 @@
     </row>
     <row r="107" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A107" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B107" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15499,7 +15506,7 @@
     </row>
     <row r="111" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A111" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B111" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16318,7 +16325,7 @@
     </row>
     <row r="118" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A118" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B118" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16552,7 +16559,7 @@
     </row>
     <row r="120" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A120" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B120" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16669,7 +16676,7 @@
     </row>
     <row r="121" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A121" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B121" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16903,7 +16910,7 @@
     </row>
     <row r="123" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A123" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B123" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17137,7 +17144,7 @@
     </row>
     <row r="125" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A125" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B125" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17371,7 +17378,7 @@
     </row>
     <row r="127" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A127" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B127" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17488,7 +17495,7 @@
     </row>
     <row r="128" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A128" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B128" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17605,7 +17612,7 @@
     </row>
     <row r="129" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A129" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B129" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17839,7 +17846,7 @@
     </row>
     <row r="131" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A131" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B131" s="9" t="str">
         <f t="shared" ref="B131:B146" si="54">LEFT(A131,3)</f>
@@ -18073,7 +18080,7 @@
     </row>
     <row r="133" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A133" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B133" s="9" t="str">
         <f t="shared" si="54"/>
@@ -18307,7 +18314,7 @@
     </row>
     <row r="135" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A135" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B135" s="9" t="str">
         <f t="shared" si="54"/>
@@ -18424,7 +18431,7 @@
     </row>
     <row r="136" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A136" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B136" s="9" t="str">
         <f t="shared" si="54"/>
@@ -18541,7 +18548,7 @@
     </row>
     <row r="137" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A137" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B137" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19009,7 +19016,7 @@
     </row>
     <row r="141" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A141" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B141" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19243,7 +19250,7 @@
     </row>
     <row r="143" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A143" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B143" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19360,7 +19367,7 @@
     </row>
     <row r="144" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A144" s="12" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B144" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19477,7 +19484,7 @@
     </row>
     <row r="145" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A145" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B145" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19714,7 +19721,7 @@
         <v>200</v>
       </c>
       <c r="B147" s="9" t="str">
-        <f t="shared" ref="B147" si="76">LEFT(A147,3)</f>
+        <f t="shared" ref="B147:B149" si="76">LEFT(A147,3)</f>
         <v>LDR</v>
       </c>
       <c r="C147" s="9">
@@ -19830,19 +19837,235 @@
       <c r="A148" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="M148"/>
-      <c r="N148"/>
-      <c r="O148"/>
-      <c r="P148"/>
+      <c r="B148" s="9" t="str">
+        <f t="shared" si="76"/>
+        <v>OUT</v>
+      </c>
+      <c r="C148" s="9">
+        <f t="shared" ref="C148:C149" si="99">LEN(A148)-LEN(SUBSTITUTE(A148,",",""))</f>
+        <v>1</v>
+      </c>
+      <c r="D148" s="8">
+        <f t="shared" ref="D148:D149" si="100">IFERROR(FIND(" ",A148),LEN(A148)+1)</f>
+        <v>4</v>
+      </c>
+      <c r="E148" s="8">
+        <f t="shared" ref="E148:E149" si="101">IFERROR(FIND(",",A148,1),LEN(A148)+1)</f>
+        <v>6</v>
+      </c>
+      <c r="F148" s="8">
+        <f t="shared" ref="F148:F149" si="102">IFERROR(FIND(",",$A148,E148+1),LEN(A148)+1)</f>
+        <v>8</v>
+      </c>
+      <c r="G148" s="8">
+        <f t="shared" ref="G148:G149" si="103">IFERROR(FIND(",",$A148,F148+1),H148)</f>
+        <v>8</v>
+      </c>
+      <c r="H148" s="8">
+        <f t="shared" ref="H148:H149" si="104">IFERROR(FIND("(",A148),LEN(A148)+1)</f>
+        <v>8</v>
+      </c>
+      <c r="I148" s="9" t="str">
+        <f t="shared" ref="I148:I149" si="105">IF(EXACT(A148, "HLT"), 0, MID(A148,D148+1,1))</f>
+        <v>3</v>
+      </c>
+      <c r="J148" s="9" t="str">
+        <f t="shared" ref="J148:J149" si="106">IFERROR(MID($A148,E148+1,F148-(E148+1)),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K148" s="9">
+        <f t="shared" ref="K148:K149" si="107">IFERROR(MID($A148,F148+1,G148-(F148+1)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L148" s="9">
+        <f t="shared" ref="L148:L149" si="108">IFERROR(MID($A148,G148+1,IFERROR(H148-G148-1, 20)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M148" s="22">
+        <f>VLOOKUP($B148,'Conversion to binary Key'!$D:$I,2,0)</f>
+        <v>110010</v>
+      </c>
+      <c r="N148" s="22" t="str">
+        <f>VLOOKUP($B148,'Conversion to binary Key'!$D:$I,3,0)</f>
+        <v>00</v>
+      </c>
+      <c r="O148" s="22" t="str">
+        <f>VLOOKUP($B148,'Conversion to binary Key'!$D:$I,4,0)</f>
+        <v>00000000</v>
+      </c>
+      <c r="P148" s="22" t="str">
+        <f>VLOOKUP($B148,'Conversion to binary Key'!$D:$I,5,0)</f>
+        <v/>
+      </c>
+      <c r="Q148" s="22" t="str">
+        <f>VLOOKUP($B148,'Conversion to binary Key'!$D:$I,6,0)</f>
+        <v/>
+      </c>
+      <c r="R148" s="17">
+        <f t="shared" ref="R148:R149" si="109">M148</f>
+        <v>110010</v>
+      </c>
+      <c r="S148" s="25" t="str">
+        <f t="shared" ref="S148:S149" si="110">IF(ISNUMBER(SEARCH("binary", I148)),MID(I148, 8, 5),DEC2BIN(I148))</f>
+        <v>11</v>
+      </c>
+      <c r="T148" s="25" t="str">
+        <f t="shared" ref="T148:T149" si="111">IF(ISNUMBER(SEARCH("binary", J148)),MID(J148, 8, 5),DEC2BIN(J148))</f>
+        <v>1</v>
+      </c>
+      <c r="U148" s="25" t="str">
+        <f t="shared" ref="U148:U149" si="112">IF(ISNUMBER(SEARCH("binary", K148)),MID(K148, 8, 5),DEC2BIN(K148))</f>
+        <v>0</v>
+      </c>
+      <c r="V148" s="25" t="str">
+        <f t="shared" ref="V148:V149" si="113">IF(ISNUMBER(SEARCH("binary", L148)),MID(L148, 8, 5),DEC2BIN(L148))</f>
+        <v>0</v>
+      </c>
+      <c r="W148" s="15">
+        <f t="shared" ref="W148:W149" si="114">R148</f>
+        <v>110010</v>
+      </c>
+      <c r="X148" s="10" t="str">
+        <f t="shared" ref="X148:X149" si="115">TEXT(S148,N148)</f>
+        <v>11</v>
+      </c>
+      <c r="Y148" s="10" t="str">
+        <f t="shared" ref="Y148:Y149" si="116">TEXT(T148,O148)</f>
+        <v>00000001</v>
+      </c>
+      <c r="Z148" s="10" t="str">
+        <f t="shared" ref="Z148:Z149" si="117">TEXT(U148,P148)</f>
+        <v/>
+      </c>
+      <c r="AA148" s="10" t="str">
+        <f t="shared" ref="AA148:AA149" si="118">TEXT(V148,Q148)</f>
+        <v/>
+      </c>
+      <c r="AB148" s="11" t="str">
+        <f t="shared" ref="AB148:AB149" si="119">W148&amp;X148&amp;Y148&amp;Z148&amp;AA148</f>
+        <v>1100101100000001</v>
+      </c>
+      <c r="AC148" s="10">
+        <f t="shared" ref="AC148:AC149" si="120">LEN(AB148)</f>
+        <v>16</v>
+      </c>
     </row>
     <row r="149" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A149" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="M149"/>
-      <c r="N149"/>
-      <c r="O149"/>
-      <c r="P149"/>
+      <c r="B149" s="9" t="str">
+        <f t="shared" si="76"/>
+        <v>HLT</v>
+      </c>
+      <c r="C149" s="9">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="D149" s="8">
+        <f t="shared" si="100"/>
+        <v>4</v>
+      </c>
+      <c r="E149" s="8">
+        <f t="shared" si="101"/>
+        <v>4</v>
+      </c>
+      <c r="F149" s="8">
+        <f t="shared" si="102"/>
+        <v>4</v>
+      </c>
+      <c r="G149" s="8">
+        <f t="shared" si="103"/>
+        <v>4</v>
+      </c>
+      <c r="H149" s="8">
+        <f t="shared" si="104"/>
+        <v>4</v>
+      </c>
+      <c r="I149" s="9">
+        <f t="shared" si="105"/>
+        <v>0</v>
+      </c>
+      <c r="J149" s="9">
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+      <c r="K149" s="9">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="L149" s="9">
+        <f t="shared" si="108"/>
+        <v>0</v>
+      </c>
+      <c r="M149" s="22" t="str">
+        <f>VLOOKUP($B149,'Conversion to binary Key'!$D:$I,2,0)</f>
+        <v>000000</v>
+      </c>
+      <c r="N149" s="22" t="str">
+        <f>VLOOKUP($B149,'Conversion to binary Key'!$D:$I,3,0)</f>
+        <v>0000</v>
+      </c>
+      <c r="O149" s="22" t="str">
+        <f>VLOOKUP($B149,'Conversion to binary Key'!$D:$I,4,0)</f>
+        <v>000000</v>
+      </c>
+      <c r="P149" s="22" t="str">
+        <f>VLOOKUP($B149,'Conversion to binary Key'!$D:$I,5,0)</f>
+        <v/>
+      </c>
+      <c r="Q149" s="22" t="str">
+        <f>VLOOKUP($B149,'Conversion to binary Key'!$D:$I,6,0)</f>
+        <v/>
+      </c>
+      <c r="R149" s="17" t="str">
+        <f t="shared" si="109"/>
+        <v>000000</v>
+      </c>
+      <c r="S149" s="25" t="str">
+        <f t="shared" si="110"/>
+        <v>0</v>
+      </c>
+      <c r="T149" s="25" t="str">
+        <f t="shared" si="111"/>
+        <v>0</v>
+      </c>
+      <c r="U149" s="25" t="str">
+        <f t="shared" si="112"/>
+        <v>0</v>
+      </c>
+      <c r="V149" s="25" t="str">
+        <f t="shared" si="113"/>
+        <v>0</v>
+      </c>
+      <c r="W149" s="15" t="str">
+        <f t="shared" si="114"/>
+        <v>000000</v>
+      </c>
+      <c r="X149" s="10" t="str">
+        <f t="shared" si="115"/>
+        <v>0000</v>
+      </c>
+      <c r="Y149" s="10" t="str">
+        <f t="shared" si="116"/>
+        <v>000000</v>
+      </c>
+      <c r="Z149" s="10" t="str">
+        <f t="shared" si="117"/>
+        <v/>
+      </c>
+      <c r="AA149" s="10" t="str">
+        <f t="shared" si="118"/>
+        <v/>
+      </c>
+      <c r="AB149" s="11" t="str">
+        <f t="shared" si="119"/>
+        <v>0000000000000000</v>
+      </c>
+      <c r="AC149" s="10">
+        <f t="shared" si="120"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="150" spans="1:29" x14ac:dyDescent="0.3">
       <c r="M150"/>
@@ -20440,8 +20663,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AC146"/>
-  <conditionalFormatting sqref="AC2:AC147">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="notEqual">
+  <conditionalFormatting sqref="AC2:AC149">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="notEqual">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Program 1 fixes, cont.
</commit_message>
<xml_diff>
--- a/Convert to Binary_v3 - Program 1.xlsx
+++ b/Convert to Binary_v3 - Program 1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Program1.txt" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="322">
   <si>
     <t>LDX 1,0,29</t>
   </si>
@@ -520,9 +520,6 @@
     <t>LDA 3,1,0,30(a)</t>
   </si>
   <si>
-    <t>Array starts at address a=190</t>
-  </si>
-  <si>
     <t>STR 3,1,0,26(i)</t>
   </si>
   <si>
@@ -562,9 +559,6 @@
     <t>Add 1 to Array Element Address by loading the Array Element Address contents into R3; ARRAY INPUT FOR LOOP START</t>
   </si>
   <si>
-    <t>STR 3,1,1,26(i)</t>
-  </si>
-  <si>
     <t>Then storing the R3 contents back into the Array Element Address</t>
   </si>
   <si>
@@ -634,6 +628,9 @@
     <t>Set R0 contents back to 0</t>
   </si>
   <si>
+    <t>SOB 1,2,0,0(aifls)</t>
+  </si>
+  <si>
     <t>Subtract 1 from R1 and if &gt; 0, branch back to ARRAY INPUT FOR LOOP START</t>
   </si>
   <si>
@@ -955,9 +952,6 @@
     <t>JCC 1,3,0,16(hnd)</t>
   </si>
   <si>
-    <t>STR 3,1,0,21(d)</t>
-  </si>
-  <si>
     <t>SOB 1,3,0,9(cmfls)</t>
   </si>
   <si>
@@ -988,9 +982,6 @@
     <t>JZ 2,3,0,26(g1p)</t>
   </si>
   <si>
-    <t>SOB 1,2,0,1(aifls)</t>
-  </si>
-  <si>
     <t>Memory address d=189 (decimal) stores the minimum difference between the number to try to match and the closest array value AKA Min Diff Address (defaults to 16 ones)</t>
   </si>
   <si>
@@ -998,6 +989,12 @@
   </si>
   <si>
     <t>x changed from what I thought, but leaving an instruction here so addresses won't be off</t>
+  </si>
+  <si>
+    <t>LDA 3,1,0,29(a)</t>
+  </si>
+  <si>
+    <t>Array starts at address a=190 (but loop increments first so store 189 initially)</t>
   </si>
 </sst>
 </file>
@@ -1538,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" workbookViewId="0">
-      <selection sqref="A1:A148"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1591,12 +1588,12 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1614,15 +1611,15 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1656,7 +1653,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D17" t="s">
         <v>152</v>
@@ -1669,7 +1666,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D19" t="s">
         <v>153</v>
@@ -1682,7 +1679,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F21" t="s">
         <v>155</v>
@@ -1698,18 +1695,18 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E23" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1722,7 +1719,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1732,7 +1729,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1753,42 +1750,42 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>320</v>
       </c>
       <c r="E31" t="s">
-        <v>163</v>
+        <v>321</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="G32" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>163</v>
+      </c>
+      <c r="E33" t="s">
         <v>164</v>
-      </c>
-      <c r="E33" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>165</v>
+      </c>
+      <c r="E34" t="s">
         <v>166</v>
-      </c>
-      <c r="E34" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>167</v>
+      </c>
+      <c r="E35" t="s">
         <v>168</v>
-      </c>
-      <c r="E35" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -1796,7 +1793,7 @@
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -1804,7 +1801,7 @@
         <v>4</v>
       </c>
       <c r="F37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -1814,18 +1811,18 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>171</v>
+      </c>
+      <c r="E39" t="s">
         <v>172</v>
-      </c>
-      <c r="E39" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>215</v>
+      </c>
+      <c r="E40" t="s">
         <v>175</v>
-      </c>
-      <c r="E40" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -1838,129 +1835,129 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="E42" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G43" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E44" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>292</v>
+      </c>
+      <c r="D45" t="s">
         <v>293</v>
-      </c>
-      <c r="D45" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>287</v>
+      </c>
+      <c r="D46" t="s">
         <v>288</v>
-      </c>
-      <c r="D46" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E47" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G48" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E49" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E51" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E52" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G54" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D55" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E56" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E57" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -1968,134 +1965,134 @@
         <v>4</v>
       </c>
       <c r="F59" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>319</v>
+        <v>199</v>
       </c>
       <c r="D60" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G61" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E62" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D63" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E64" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G65" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E66" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E68" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G70" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E71" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>304</v>
+      </c>
+      <c r="G72" t="s">
         <v>305</v>
-      </c>
-      <c r="G72" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>206</v>
+      </c>
+      <c r="E73" t="s">
         <v>207</v>
-      </c>
-      <c r="E73" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E74" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E76" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -2103,41 +2100,41 @@
         <v>162</v>
       </c>
       <c r="E77" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>211</v>
+      </c>
+      <c r="E80" t="s">
         <v>212</v>
-      </c>
-      <c r="E80" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>213</v>
+      </c>
+      <c r="E81" t="s">
         <v>214</v>
-      </c>
-      <c r="E81" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
+        <v>215</v>
+      </c>
+      <c r="E82" t="s">
         <v>216</v>
-      </c>
-      <c r="E82" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -2150,127 +2147,127 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E84" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>217</v>
+      </c>
+      <c r="E85" t="s">
         <v>218</v>
-      </c>
-      <c r="E85" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
+        <v>219</v>
+      </c>
+      <c r="E86" t="s">
         <v>220</v>
-      </c>
-      <c r="E86" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D87" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E88" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E89" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
+        <v>224</v>
+      </c>
+      <c r="E90" t="s">
         <v>225</v>
-      </c>
-      <c r="E90" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
+        <v>226</v>
+      </c>
+      <c r="E91" t="s">
         <v>227</v>
-      </c>
-      <c r="E91" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D92" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E93" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>308</v>
+        <v>173</v>
       </c>
       <c r="E94" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
+        <v>231</v>
+      </c>
+      <c r="E95" t="s">
         <v>232</v>
-      </c>
-      <c r="E95" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D96" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
+        <v>234</v>
+      </c>
+      <c r="E97" t="s">
         <v>235</v>
-      </c>
-      <c r="E97" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F98" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -2278,7 +2275,7 @@
         <v>144</v>
       </c>
       <c r="E100" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -2288,10 +2285,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>238</v>
+      </c>
+      <c r="E102" t="s">
         <v>239</v>
-      </c>
-      <c r="E102" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -2299,7 +2296,7 @@
         <v>3</v>
       </c>
       <c r="E103" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -2307,86 +2304,86 @@
         <v>9</v>
       </c>
       <c r="E104" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G105" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E106" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E107" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G109" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E110" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E111" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G113" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E114" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
@@ -2394,15 +2391,15 @@
         <v>10</v>
       </c>
       <c r="F116" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
+        <v>249</v>
+      </c>
+      <c r="E117" t="s">
         <v>250</v>
-      </c>
-      <c r="E117" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
@@ -2410,23 +2407,23 @@
         <v>11</v>
       </c>
       <c r="G118" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D119" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
+        <v>253</v>
+      </c>
+      <c r="G120" t="s">
         <v>254</v>
-      </c>
-      <c r="G120" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
@@ -2434,28 +2431,28 @@
         <v>12</v>
       </c>
       <c r="F121" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
+        <v>256</v>
+      </c>
+      <c r="E122" t="s">
         <v>257</v>
-      </c>
-      <c r="E122" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E123" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
@@ -2463,31 +2460,31 @@
         <v>11</v>
       </c>
       <c r="G125" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D126" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D127" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G128" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -2495,28 +2492,28 @@
         <v>12</v>
       </c>
       <c r="F129" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
+        <v>264</v>
+      </c>
+      <c r="E130" t="s">
         <v>265</v>
-      </c>
-      <c r="E130" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E131" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
@@ -2524,31 +2521,31 @@
         <v>11</v>
       </c>
       <c r="G133" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D134" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D135" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G136" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
@@ -2556,7 +2553,7 @@
         <v>12</v>
       </c>
       <c r="F137" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
@@ -2564,20 +2561,20 @@
         <v>3</v>
       </c>
       <c r="E138" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E139" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
@@ -2585,52 +2582,52 @@
         <v>11</v>
       </c>
       <c r="G141" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D142" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D143" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G144" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G145" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E146" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
@@ -2638,7 +2635,7 @@
         <v>13</v>
       </c>
       <c r="H148" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -2650,11 +2647,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD248"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2986,7 +2983,7 @@
         <v>000101</v>
       </c>
       <c r="AB3" s="11" t="str">
-        <f t="shared" ref="AB3:AB66" si="29">W3&amp;X3&amp;Y3&amp;Z3&amp;AA3</f>
+        <f>W3&amp;X3&amp;Y3&amp;Z3&amp;AA3</f>
         <v>0110011111000101</v>
       </c>
       <c r="AC3" s="10">
@@ -3103,7 +3100,7 @@
         <v/>
       </c>
       <c r="AB4" s="11" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="AB3:AB66" si="29">W4&amp;X4&amp;Y4&amp;Z4&amp;AA4</f>
         <v>0001101100000000</v>
       </c>
       <c r="AC4" s="10">
@@ -3464,7 +3461,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B8" s="9" t="str">
         <f t="shared" si="8"/>
@@ -3581,7 +3578,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B9" s="9" t="str">
         <f t="shared" si="8"/>
@@ -3932,7 +3929,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B12" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4049,7 +4046,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B13" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4634,7 +4631,7 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B18" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4868,7 +4865,7 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B20" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5102,7 +5099,7 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B22" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5336,7 +5333,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B24" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5453,7 +5450,7 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B25" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5687,7 +5684,7 @@
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B27" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5921,7 +5918,7 @@
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B29" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6272,7 +6269,7 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>162</v>
+        <v>320</v>
       </c>
       <c r="B32" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6316,7 +6313,7 @@
       </c>
       <c r="L32" s="9" t="str">
         <f t="shared" si="18"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M32" s="22" t="str">
         <f>VLOOKUP($B32,'Conversion to binary Key'!$D:$I,2,0)</f>
@@ -6356,7 +6353,7 @@
       </c>
       <c r="V32" s="25" t="str">
         <f t="shared" si="23"/>
-        <v>11110</v>
+        <v>11101</v>
       </c>
       <c r="W32" s="15" t="str">
         <f t="shared" si="24"/>
@@ -6376,11 +6373,11 @@
       </c>
       <c r="AA32" s="10" t="str">
         <f t="shared" si="28"/>
-        <v>11110</v>
+        <v>11101</v>
       </c>
       <c r="AB32" s="11" t="str">
         <f t="shared" si="29"/>
-        <v>0000111101011110</v>
+        <v>0000111101011101</v>
       </c>
       <c r="AC32" s="10">
         <f t="shared" si="7"/>
@@ -6389,7 +6386,7 @@
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B33" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6506,7 +6503,7 @@
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B34" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6623,7 +6620,7 @@
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B35" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6740,7 +6737,7 @@
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B36" s="9" t="str">
         <f t="shared" si="8"/>
@@ -7208,7 +7205,7 @@
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B40" s="9" t="str">
         <f t="shared" si="8"/>
@@ -7325,7 +7322,7 @@
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
-        <v>175</v>
+        <v>215</v>
       </c>
       <c r="B41" s="9" t="str">
         <f t="shared" si="8"/>
@@ -7365,7 +7362,7 @@
       </c>
       <c r="K41" s="9" t="str">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L41" s="9" t="str">
         <f t="shared" si="18"/>
@@ -7405,7 +7402,7 @@
       </c>
       <c r="U41" s="25" t="str">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V41" s="25" t="str">
         <f t="shared" si="23"/>
@@ -7425,7 +7422,7 @@
       </c>
       <c r="Z41" s="10" t="str">
         <f t="shared" si="27"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA41" s="10" t="str">
         <f t="shared" si="28"/>
@@ -7433,7 +7430,7 @@
       </c>
       <c r="AB41" s="11" t="str">
         <f t="shared" si="29"/>
-        <v>0000011101111010</v>
+        <v>0000011101011010</v>
       </c>
       <c r="AC41" s="10">
         <f t="shared" si="7"/>
@@ -7559,7 +7556,7 @@
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="B43" s="9" t="str">
         <f t="shared" si="8"/>
@@ -7599,7 +7596,7 @@
       </c>
       <c r="K43" s="9" t="str">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L43" s="9" t="str">
         <f t="shared" si="18"/>
@@ -7639,7 +7636,7 @@
       </c>
       <c r="U43" s="25" t="str">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V43" s="25" t="str">
         <f t="shared" si="23"/>
@@ -7659,7 +7656,7 @@
       </c>
       <c r="Z43" s="10" t="str">
         <f t="shared" si="27"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA43" s="10" t="str">
         <f t="shared" si="28"/>
@@ -7667,7 +7664,7 @@
       </c>
       <c r="AB43" s="11" t="str">
         <f t="shared" si="29"/>
-        <v>0000101101111010</v>
+        <v>0000101101011010</v>
       </c>
       <c r="AC43" s="10">
         <f t="shared" si="7"/>
@@ -7676,7 +7673,7 @@
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B44" s="9" t="str">
         <f t="shared" si="8"/>
@@ -7793,7 +7790,7 @@
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B45" s="9" t="str">
         <f t="shared" si="8"/>
@@ -7910,7 +7907,7 @@
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B46" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8027,7 +8024,7 @@
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B47" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8144,7 +8141,7 @@
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B48" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8261,7 +8258,7 @@
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B49" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8378,7 +8375,7 @@
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B50" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8495,7 +8492,7 @@
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B51" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8612,7 +8609,7 @@
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B52" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8729,7 +8726,7 @@
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B53" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8846,7 +8843,7 @@
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B54" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8963,7 +8960,7 @@
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B55" s="9" t="str">
         <f t="shared" si="8"/>
@@ -9080,7 +9077,7 @@
     </row>
     <row r="56" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B56" s="9" t="str">
         <f t="shared" si="8"/>
@@ -9197,7 +9194,7 @@
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A57" s="12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B57" s="9" t="str">
         <f t="shared" si="8"/>
@@ -9314,7 +9311,7 @@
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A58" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B58" s="9" t="str">
         <f t="shared" si="8"/>
@@ -9431,7 +9428,7 @@
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B59" s="9" t="str">
         <f t="shared" si="8"/>
@@ -9665,7 +9662,7 @@
     </row>
     <row r="61" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A61" s="12" t="s">
-        <v>319</v>
+        <v>199</v>
       </c>
       <c r="B61" s="9" t="str">
         <f t="shared" si="8"/>
@@ -9709,7 +9706,7 @@
       </c>
       <c r="L61" s="9" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M61" s="22" t="str">
         <f>VLOOKUP($B61,'Conversion to binary Key'!$D:$I,2,0)</f>
@@ -9749,7 +9746,7 @@
       </c>
       <c r="V61" s="25" t="str">
         <f t="shared" si="23"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W61" s="15" t="str">
         <f t="shared" si="24"/>
@@ -9769,11 +9766,11 @@
       </c>
       <c r="AA61" s="10" t="str">
         <f t="shared" si="28"/>
-        <v>00001</v>
+        <v>00000</v>
       </c>
       <c r="AB61" s="11" t="str">
         <f t="shared" si="29"/>
-        <v>0011100110000001</v>
+        <v>0011100110000000</v>
       </c>
       <c r="AC61" s="10">
         <f t="shared" si="7"/>
@@ -9782,7 +9779,7 @@
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A62" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B62" s="9" t="str">
         <f t="shared" si="8"/>
@@ -9899,7 +9896,7 @@
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A63" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B63" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10016,7 +10013,7 @@
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B64" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10133,7 +10130,7 @@
     </row>
     <row r="65" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B65" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10250,7 +10247,7 @@
     </row>
     <row r="66" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A66" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B66" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10367,7 +10364,7 @@
     </row>
     <row r="67" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A67" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B67" s="9" t="str">
         <f t="shared" ref="B67:B130" si="31">LEFT(A67,3)</f>
@@ -10484,7 +10481,7 @@
     </row>
     <row r="68" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B68" s="9" t="str">
         <f t="shared" si="31"/>
@@ -10601,7 +10598,7 @@
     </row>
     <row r="69" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A69" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B69" s="9" t="str">
         <f t="shared" si="31"/>
@@ -10718,7 +10715,7 @@
     </row>
     <row r="70" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A70" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B70" s="9" t="str">
         <f t="shared" si="31"/>
@@ -10835,7 +10832,7 @@
     </row>
     <row r="71" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A71" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B71" s="9" t="str">
         <f t="shared" si="31"/>
@@ -10952,7 +10949,7 @@
     </row>
     <row r="72" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A72" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B72" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11069,7 +11066,7 @@
     </row>
     <row r="73" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B73" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11186,7 +11183,7 @@
     </row>
     <row r="74" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A74" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B74" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11303,7 +11300,7 @@
     </row>
     <row r="75" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A75" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B75" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11420,7 +11417,7 @@
     </row>
     <row r="76" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B76" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11537,7 +11534,7 @@
     </row>
     <row r="77" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A77" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B77" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11771,7 +11768,7 @@
     </row>
     <row r="79" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A79" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B79" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11888,7 +11885,7 @@
     </row>
     <row r="80" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A80" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B80" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12005,7 +12002,7 @@
     </row>
     <row r="81" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A81" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B81" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12122,7 +12119,7 @@
     </row>
     <row r="82" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A82" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B82" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12239,7 +12236,7 @@
     </row>
     <row r="83" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A83" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B83" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12473,7 +12470,7 @@
     </row>
     <row r="85" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A85" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B85" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12590,7 +12587,7 @@
     </row>
     <row r="86" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A86" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B86" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12707,7 +12704,7 @@
     </row>
     <row r="87" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A87" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B87" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12824,7 +12821,7 @@
     </row>
     <row r="88" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A88" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B88" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12941,7 +12938,7 @@
     </row>
     <row r="89" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B89" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13058,7 +13055,7 @@
     </row>
     <row r="90" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A90" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B90" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13175,7 +13172,7 @@
     </row>
     <row r="91" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A91" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B91" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13292,7 +13289,7 @@
     </row>
     <row r="92" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A92" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B92" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13409,7 +13406,7 @@
     </row>
     <row r="93" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A93" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B93" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13526,7 +13523,7 @@
     </row>
     <row r="94" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A94" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B94" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13643,7 +13640,7 @@
     </row>
     <row r="95" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A95" s="12" t="s">
-        <v>308</v>
+        <v>173</v>
       </c>
       <c r="B95" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13687,7 +13684,7 @@
       </c>
       <c r="L95" s="9" t="str">
         <f t="shared" si="41"/>
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="M95" s="22" t="str">
         <f>VLOOKUP($B95,'Conversion to binary Key'!$D:$I,2,0)</f>
@@ -13727,7 +13724,7 @@
       </c>
       <c r="V95" s="25" t="str">
         <f t="shared" si="46"/>
-        <v>10101</v>
+        <v>11101</v>
       </c>
       <c r="W95" s="15" t="str">
         <f t="shared" si="47"/>
@@ -13747,11 +13744,11 @@
       </c>
       <c r="AA95" s="10" t="str">
         <f t="shared" si="51"/>
-        <v>10101</v>
+        <v>11101</v>
       </c>
       <c r="AB95" s="11" t="str">
         <f t="shared" si="52"/>
-        <v>0000101101010101</v>
+        <v>0000101101011101</v>
       </c>
       <c r="AC95" s="10">
         <f t="shared" si="30"/>
@@ -13760,7 +13757,7 @@
     </row>
     <row r="96" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A96" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B96" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13877,7 +13874,7 @@
     </row>
     <row r="97" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B97" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13994,7 +13991,7 @@
     </row>
     <row r="98" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A98" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B98" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14111,7 +14108,7 @@
     </row>
     <row r="99" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A99" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B99" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14228,7 +14225,7 @@
     </row>
     <row r="100" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B100" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14579,7 +14576,7 @@
     </row>
     <row r="103" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B103" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14930,7 +14927,7 @@
     </row>
     <row r="106" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A106" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B106" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15047,7 +15044,7 @@
     </row>
     <row r="107" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A107" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B107" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15164,7 +15161,7 @@
     </row>
     <row r="108" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A108" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B108" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15281,7 +15278,7 @@
     </row>
     <row r="109" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A109" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B109" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15398,7 +15395,7 @@
     </row>
     <row r="110" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A110" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B110" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15515,7 +15512,7 @@
     </row>
     <row r="111" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A111" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B111" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15632,7 +15629,7 @@
     </row>
     <row r="112" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A112" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B112" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15749,7 +15746,7 @@
     </row>
     <row r="113" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A113" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B113" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15866,7 +15863,7 @@
     </row>
     <row r="114" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A114" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B114" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15983,7 +15980,7 @@
     </row>
     <row r="115" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A115" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B115" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16100,7 +16097,7 @@
     </row>
     <row r="116" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A116" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B116" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16334,7 +16331,7 @@
     </row>
     <row r="118" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A118" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B118" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16568,7 +16565,7 @@
     </row>
     <row r="120" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A120" s="12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B120" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16685,7 +16682,7 @@
     </row>
     <row r="121" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A121" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B121" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16919,7 +16916,7 @@
     </row>
     <row r="123" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A123" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B123" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17036,7 +17033,7 @@
     </row>
     <row r="124" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A124" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B124" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17153,7 +17150,7 @@
     </row>
     <row r="125" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A125" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B125" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17387,7 +17384,7 @@
     </row>
     <row r="127" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A127" s="12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B127" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17504,7 +17501,7 @@
     </row>
     <row r="128" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A128" s="12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B128" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17621,7 +17618,7 @@
     </row>
     <row r="129" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A129" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B129" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17855,7 +17852,7 @@
     </row>
     <row r="131" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A131" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B131" s="9" t="str">
         <f t="shared" ref="B131:B146" si="54">LEFT(A131,3)</f>
@@ -17972,7 +17969,7 @@
     </row>
     <row r="132" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A132" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B132" s="9" t="str">
         <f t="shared" si="54"/>
@@ -18089,7 +18086,7 @@
     </row>
     <row r="133" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A133" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B133" s="9" t="str">
         <f t="shared" si="54"/>
@@ -18323,7 +18320,7 @@
     </row>
     <row r="135" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A135" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B135" s="9" t="str">
         <f t="shared" si="54"/>
@@ -18440,7 +18437,7 @@
     </row>
     <row r="136" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A136" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B136" s="9" t="str">
         <f t="shared" si="54"/>
@@ -18557,7 +18554,7 @@
     </row>
     <row r="137" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A137" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B137" s="9" t="str">
         <f t="shared" si="54"/>
@@ -18908,7 +18905,7 @@
     </row>
     <row r="140" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A140" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B140" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19025,7 +19022,7 @@
     </row>
     <row r="141" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A141" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B141" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19259,7 +19256,7 @@
     </row>
     <row r="143" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A143" s="12" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B143" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19376,7 +19373,7 @@
     </row>
     <row r="144" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A144" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B144" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19493,7 +19490,7 @@
     </row>
     <row r="145" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A145" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B145" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19610,7 +19607,7 @@
     </row>
     <row r="146" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A146" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B146" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19727,7 +19724,7 @@
     </row>
     <row r="147" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A147" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B147" s="9" t="str">
         <f t="shared" ref="B147:B149" si="76">LEFT(A147,3)</f>
@@ -19844,7 +19841,7 @@
     </row>
     <row r="148" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A148" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B148" s="9" t="str">
         <f t="shared" si="76"/>

</xml_diff>

<commit_message>
final, working Program 1
</commit_message>
<xml_diff>
--- a/Convert to Binary_v3 - Program 1.xlsx
+++ b/Convert to Binary_v3 - Program 1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Program1.txt" sheetId="1" r:id="rId1"/>
@@ -739,9 +739,6 @@
     <t>Address 29 should still have z stored in it; PRINT CLOSEST MATCH START</t>
   </si>
   <si>
-    <t>z = z + 40 = 148 (decimal) so can reach even later addresses</t>
-  </si>
-  <si>
     <t>Set X3 to z (passes through address 29)</t>
   </si>
   <si>
@@ -886,9 +883,6 @@
     <t>SIR 3,1</t>
   </si>
   <si>
-    <t>AIR 3,10</t>
-  </si>
-  <si>
     <t>Memory address n=185 stores the bit string that represents a newline character, 1010101010101010 (don't use ASCII code since that could be mistaken for a number)</t>
   </si>
   <si>
@@ -904,9 +898,6 @@
     <t>JMA 2,0,21(mis)</t>
   </si>
   <si>
-    <t>JMA 3,0,10(cd)</t>
-  </si>
-  <si>
     <t>JCC 1,2,0,7(paid)</t>
   </si>
   <si>
@@ -925,12 +916,6 @@
     <t>Multiply R0 contents by 10 (decimal, stored in R2) to move it to the tens place; PROCESS MATCH INPUT DIGIT</t>
   </si>
   <si>
-    <t>JCC 1,3,0,14(ncmf)</t>
-  </si>
-  <si>
-    <t>JMA 3,0,16(ne)</t>
-  </si>
-  <si>
     <t>Set X3 to z=102 to aid with jumping to later addresses</t>
   </si>
   <si>
@@ -995,6 +980,21 @@
   </si>
   <si>
     <t>Array starts at address a=190 (but loop increments first so store 189 initially)</t>
+  </si>
+  <si>
+    <t>JMA 3,0,18(cd)</t>
+  </si>
+  <si>
+    <t>JMA 3,0,23(ne)</t>
+  </si>
+  <si>
+    <t>JCC 1,3,0,21(ncmf)</t>
+  </si>
+  <si>
+    <t>z = z + 46 = 148 (decimal) so can reach even later addresses</t>
+  </si>
+  <si>
+    <t>AIR 3,16</t>
   </si>
 </sst>
 </file>
@@ -1215,21 +1215,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1535,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView topLeftCell="A120" workbookViewId="0">
+      <selection sqref="A1:A148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1588,12 +1574,12 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1611,15 +1597,15 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F11" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1653,7 +1639,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D17" t="s">
         <v>152</v>
@@ -1666,7 +1652,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D19" t="s">
         <v>153</v>
@@ -1679,7 +1665,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F21" t="s">
         <v>155</v>
@@ -1698,15 +1684,15 @@
         <v>173</v>
       </c>
       <c r="E23" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C24" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1719,7 +1705,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1729,7 +1715,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1750,18 +1736,18 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E31" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="G32" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1859,18 +1845,18 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D45" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D46" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -1878,7 +1864,7 @@
         <v>167</v>
       </c>
       <c r="E47" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -1952,7 +1938,7 @@
         <v>197</v>
       </c>
       <c r="E57" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -1994,18 +1980,18 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="D63" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E64" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -2013,7 +1999,7 @@
         <v>181</v>
       </c>
       <c r="G65" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2052,7 +2038,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E71" t="s">
         <v>205</v>
@@ -2060,10 +2046,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G72" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -2105,7 +2091,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -2171,7 +2157,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D87" t="s">
         <v>221</v>
@@ -2179,7 +2165,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c r="E88" t="s">
         <v>222</v>
@@ -2211,7 +2197,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>298</v>
+        <v>319</v>
       </c>
       <c r="D92" t="s">
         <v>228</v>
@@ -2219,7 +2205,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>299</v>
+        <v>318</v>
       </c>
       <c r="E93" t="s">
         <v>229</v>
@@ -2243,7 +2229,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D96" t="s">
         <v>233</v>
@@ -2259,15 +2245,15 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F98" t="s">
-        <v>236</v>
+        <v>320</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>285</v>
+        <v>321</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -2275,7 +2261,7 @@
         <v>144</v>
       </c>
       <c r="E100" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -2285,10 +2271,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>237</v>
+      </c>
+      <c r="E102" t="s">
         <v>238</v>
-      </c>
-      <c r="E102" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -2296,7 +2282,7 @@
         <v>3</v>
       </c>
       <c r="E103" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -2304,7 +2290,7 @@
         <v>9</v>
       </c>
       <c r="E104" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
@@ -2312,15 +2298,15 @@
         <v>181</v>
       </c>
       <c r="G105" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E106" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
@@ -2328,7 +2314,7 @@
         <v>183</v>
       </c>
       <c r="E107" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
@@ -2341,15 +2327,15 @@
         <v>181</v>
       </c>
       <c r="G109" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E110" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
@@ -2357,7 +2343,7 @@
         <v>183</v>
       </c>
       <c r="E111" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
@@ -2370,7 +2356,7 @@
         <v>181</v>
       </c>
       <c r="G113" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
@@ -2378,7 +2364,7 @@
         <v>183</v>
       </c>
       <c r="E114" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
@@ -2391,15 +2377,15 @@
         <v>10</v>
       </c>
       <c r="F116" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
+        <v>248</v>
+      </c>
+      <c r="E117" t="s">
         <v>249</v>
-      </c>
-      <c r="E117" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
@@ -2407,23 +2393,23 @@
         <v>11</v>
       </c>
       <c r="G118" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="D119" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
+        <v>252</v>
+      </c>
+      <c r="G120" t="s">
         <v>253</v>
-      </c>
-      <c r="G120" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
@@ -2431,15 +2417,15 @@
         <v>12</v>
       </c>
       <c r="F121" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
+        <v>255</v>
+      </c>
+      <c r="E122" t="s">
         <v>256</v>
-      </c>
-      <c r="E122" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
@@ -2447,12 +2433,12 @@
         <v>188</v>
       </c>
       <c r="E123" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
@@ -2460,31 +2446,31 @@
         <v>11</v>
       </c>
       <c r="G125" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D126" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D127" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G128" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -2492,15 +2478,15 @@
         <v>12</v>
       </c>
       <c r="F129" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
+        <v>263</v>
+      </c>
+      <c r="E130" t="s">
         <v>264</v>
-      </c>
-      <c r="E130" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
@@ -2508,12 +2494,12 @@
         <v>188</v>
       </c>
       <c r="E131" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
@@ -2521,31 +2507,31 @@
         <v>11</v>
       </c>
       <c r="G133" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D134" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D135" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G136" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
@@ -2553,7 +2539,7 @@
         <v>12</v>
       </c>
       <c r="F137" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
@@ -2561,7 +2547,7 @@
         <v>3</v>
       </c>
       <c r="E138" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
@@ -2569,12 +2555,12 @@
         <v>188</v>
       </c>
       <c r="E139" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
@@ -2582,31 +2568,31 @@
         <v>11</v>
       </c>
       <c r="G141" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D142" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D143" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G144" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
@@ -2614,7 +2600,7 @@
         <v>191</v>
       </c>
       <c r="G145" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
@@ -2635,7 +2621,7 @@
         <v>13</v>
       </c>
       <c r="H148" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -2647,11 +2633,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD248"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A96" sqref="A96"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3461,7 +3447,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B8" s="9" t="str">
         <f t="shared" si="8"/>
@@ -3578,7 +3564,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B9" s="9" t="str">
         <f t="shared" si="8"/>
@@ -3929,7 +3915,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B12" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4046,7 +4032,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B13" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4631,7 +4617,7 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B18" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4865,7 +4851,7 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B20" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5099,7 +5085,7 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B22" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5450,7 +5436,7 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B25" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5684,7 +5670,7 @@
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B27" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5918,7 +5904,7 @@
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B29" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6269,7 +6255,7 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B32" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6386,7 +6372,7 @@
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B33" s="9" t="str">
         <f t="shared" si="8"/>
@@ -7907,7 +7893,7 @@
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B46" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8024,7 +8010,7 @@
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B47" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10013,7 +9999,7 @@
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B64" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10130,7 +10116,7 @@
     </row>
     <row r="65" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B65" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10949,7 +10935,7 @@
     </row>
     <row r="72" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A72" s="12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B72" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11066,7 +11052,7 @@
     </row>
     <row r="73" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B73" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11768,7 +11754,7 @@
     </row>
     <row r="79" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A79" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B79" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12821,7 +12807,7 @@
     </row>
     <row r="88" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A88" s="12" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="B88" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12938,7 +12924,7 @@
     </row>
     <row r="89" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c r="B89" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12978,7 +12964,7 @@
       </c>
       <c r="K89" s="9" t="str">
         <f t="shared" si="40"/>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="L89" s="9">
         <f t="shared" si="41"/>
@@ -13018,7 +13004,7 @@
       </c>
       <c r="U89" s="25" t="str">
         <f t="shared" si="45"/>
-        <v>1010</v>
+        <v>10010</v>
       </c>
       <c r="V89" s="25" t="str">
         <f t="shared" si="46"/>
@@ -13038,7 +13024,7 @@
       </c>
       <c r="Z89" s="10" t="str">
         <f t="shared" si="50"/>
-        <v>01010</v>
+        <v>10010</v>
       </c>
       <c r="AA89" s="10" t="str">
         <f t="shared" si="51"/>
@@ -13046,7 +13032,7 @@
       </c>
       <c r="AB89" s="11" t="str">
         <f t="shared" si="52"/>
-        <v>0010110011001010</v>
+        <v>0010110011010010</v>
       </c>
       <c r="AC89" s="10">
         <f t="shared" si="30"/>
@@ -13406,7 +13392,7 @@
     </row>
     <row r="93" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A93" s="12" t="s">
-        <v>298</v>
+        <v>319</v>
       </c>
       <c r="B93" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13450,7 +13436,7 @@
       </c>
       <c r="L93" s="9" t="str">
         <f t="shared" si="41"/>
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="M93" s="22" t="str">
         <f>VLOOKUP($B93,'Conversion to binary Key'!$D:$I,2,0)</f>
@@ -13490,7 +13476,7 @@
       </c>
       <c r="V93" s="25" t="str">
         <f t="shared" si="46"/>
-        <v>1110</v>
+        <v>10101</v>
       </c>
       <c r="W93" s="15" t="str">
         <f t="shared" si="47"/>
@@ -13510,11 +13496,11 @@
       </c>
       <c r="AA93" s="10" t="str">
         <f t="shared" si="51"/>
-        <v>01110</v>
+        <v>10101</v>
       </c>
       <c r="AB93" s="11" t="str">
         <f t="shared" si="52"/>
-        <v>0010100111001110</v>
+        <v>0010100111010101</v>
       </c>
       <c r="AC93" s="10">
         <f t="shared" si="30"/>
@@ -13523,7 +13509,7 @@
     </row>
     <row r="94" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A94" s="12" t="s">
-        <v>299</v>
+        <v>318</v>
       </c>
       <c r="B94" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13563,7 +13549,7 @@
       </c>
       <c r="K94" s="9" t="str">
         <f t="shared" si="40"/>
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="L94" s="9">
         <f t="shared" si="41"/>
@@ -13603,7 +13589,7 @@
       </c>
       <c r="U94" s="25" t="str">
         <f t="shared" si="45"/>
-        <v>10000</v>
+        <v>10111</v>
       </c>
       <c r="V94" s="25" t="str">
         <f t="shared" si="46"/>
@@ -13623,7 +13609,7 @@
       </c>
       <c r="Z94" s="10" t="str">
         <f t="shared" si="50"/>
-        <v>10000</v>
+        <v>10111</v>
       </c>
       <c r="AA94" s="10" t="str">
         <f t="shared" si="51"/>
@@ -13631,7 +13617,7 @@
       </c>
       <c r="AB94" s="11" t="str">
         <f t="shared" si="52"/>
-        <v>0010110011010000</v>
+        <v>0010110011010111</v>
       </c>
       <c r="AC94" s="10">
         <f t="shared" si="30"/>
@@ -13874,7 +13860,7 @@
     </row>
     <row r="97" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B97" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14108,7 +14094,7 @@
     </row>
     <row r="99" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A99" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B99" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14225,7 +14211,7 @@
     </row>
     <row r="100" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
-        <v>285</v>
+        <v>321</v>
       </c>
       <c r="B100" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14261,7 +14247,7 @@
       </c>
       <c r="J100" s="9" t="str">
         <f t="shared" si="39"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="K100" s="9">
         <f t="shared" si="40"/>
@@ -14301,7 +14287,7 @@
       </c>
       <c r="T100" s="25" t="str">
         <f t="shared" si="44"/>
-        <v>1010</v>
+        <v>10000</v>
       </c>
       <c r="U100" s="25" t="str">
         <f t="shared" si="45"/>
@@ -14321,7 +14307,7 @@
       </c>
       <c r="Y100" s="10" t="str">
         <f t="shared" si="49"/>
-        <v>00001010</v>
+        <v>00010000</v>
       </c>
       <c r="Z100" s="10" t="str">
         <f t="shared" si="50"/>
@@ -14333,7 +14319,7 @@
       </c>
       <c r="AB100" s="11" t="str">
         <f t="shared" si="52"/>
-        <v>0001101100001010</v>
+        <v>0001101100010000</v>
       </c>
       <c r="AC100" s="10">
         <f t="shared" si="30"/>
@@ -14576,7 +14562,7 @@
     </row>
     <row r="103" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B103" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15044,7 +15030,7 @@
     </row>
     <row r="107" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A107" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B107" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15512,7 +15498,7 @@
     </row>
     <row r="111" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A111" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B111" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16331,7 +16317,7 @@
     </row>
     <row r="118" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A118" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B118" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16565,7 +16551,7 @@
     </row>
     <row r="120" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A120" s="12" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B120" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16682,7 +16668,7 @@
     </row>
     <row r="121" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A121" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B121" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16916,7 +16902,7 @@
     </row>
     <row r="123" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A123" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B123" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17150,7 +17136,7 @@
     </row>
     <row r="125" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A125" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B125" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17384,7 +17370,7 @@
     </row>
     <row r="127" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A127" s="12" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B127" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17501,7 +17487,7 @@
     </row>
     <row r="128" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A128" s="12" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B128" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17618,7 +17604,7 @@
     </row>
     <row r="129" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A129" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B129" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17852,7 +17838,7 @@
     </row>
     <row r="131" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A131" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B131" s="9" t="str">
         <f t="shared" ref="B131:B146" si="54">LEFT(A131,3)</f>
@@ -18086,7 +18072,7 @@
     </row>
     <row r="133" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A133" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B133" s="9" t="str">
         <f t="shared" si="54"/>
@@ -18320,7 +18306,7 @@
     </row>
     <row r="135" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A135" s="12" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B135" s="9" t="str">
         <f t="shared" si="54"/>
@@ -18437,7 +18423,7 @@
     </row>
     <row r="136" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A136" s="12" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B136" s="9" t="str">
         <f t="shared" si="54"/>
@@ -18554,7 +18540,7 @@
     </row>
     <row r="137" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A137" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B137" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19022,7 +19008,7 @@
     </row>
     <row r="141" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A141" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B141" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19256,7 +19242,7 @@
     </row>
     <row r="143" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A143" s="12" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B143" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19373,7 +19359,7 @@
     </row>
     <row r="144" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A144" s="12" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B144" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19490,7 +19476,7 @@
     </row>
     <row r="145" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A145" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B145" s="9" t="str">
         <f t="shared" si="54"/>
@@ -20670,7 +20656,7 @@
   </sheetData>
   <autoFilter ref="A1:AC146"/>
   <conditionalFormatting sqref="AC2:AC149">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="notEqual">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
final final Program 1
</commit_message>
<xml_diff>
--- a/Convert to Binary_v3 - Program 1.xlsx
+++ b/Convert to Binary_v3 - Program 1.xlsx
@@ -733,9 +733,6 @@
     <t>Subtract 1 from R1 and if &gt; 0, branch to CLOSEST MATCH FOR LOOP START; NEXT ELEMENT</t>
   </si>
   <si>
-    <t>LDA 3,0,0,29</t>
-  </si>
-  <si>
     <t>Address 29 should still have z stored in it; PRINT CLOSEST MATCH START</t>
   </si>
   <si>
@@ -757,18 +754,12 @@
     <t>Result should be 0 in R0, 100 in R1</t>
   </si>
   <si>
-    <t>LDR 1,1,0,26(i)</t>
-  </si>
-  <si>
     <t>Move R1 contents to R0 (via Transfer Address) to prep for next MLT</t>
   </si>
   <si>
     <t>Result should be 0 in R0, 1000 in R1</t>
   </si>
   <si>
-    <t>LDR 1,1,0,29(d)</t>
-  </si>
-  <si>
     <t>Result should be 0 in R0, 10000 in R1</t>
   </si>
   <si>
@@ -796,9 +787,6 @@
     <t>Load R1 with 0, to indicate there are no more leading zeros</t>
   </si>
   <si>
-    <t>LDA 0,1,0,29(d)</t>
-  </si>
-  <si>
     <t>Load R0 with 1000 (decimal, stored in address d); GET THOUSANDS PLACE</t>
   </si>
   <si>
@@ -961,9 +949,6 @@
     <t>JZ 2,3,0,19(g10p)</t>
   </si>
   <si>
-    <t>JZ 1,3,0,25(p10p)</t>
-  </si>
-  <si>
     <t>JZ 2,3,0,26(g1p)</t>
   </si>
   <si>
@@ -995,6 +980,21 @@
   </si>
   <si>
     <t>AIR 3,16</t>
+  </si>
+  <si>
+    <t>LDR 3,0,0,29</t>
+  </si>
+  <si>
+    <t>STR 1,1,0,26(i)</t>
+  </si>
+  <si>
+    <t>STR 1,1,0,29(d)</t>
+  </si>
+  <si>
+    <t>LDR 0,1,0,29(d)</t>
+  </si>
+  <si>
+    <t>JZ 2,3,0,25(p10p)</t>
   </si>
 </sst>
 </file>
@@ -1215,21 +1215,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1521,7 +1507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView topLeftCell="A120" workbookViewId="0">
+    <sheetView topLeftCell="A119" workbookViewId="0">
       <selection sqref="A1:A148"/>
     </sheetView>
   </sheetViews>
@@ -1574,12 +1560,12 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1597,15 +1583,15 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F11" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1639,7 +1625,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D17" t="s">
         <v>152</v>
@@ -1652,7 +1638,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D19" t="s">
         <v>153</v>
@@ -1665,7 +1651,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F21" t="s">
         <v>155</v>
@@ -1684,15 +1670,15 @@
         <v>173</v>
       </c>
       <c r="E23" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C24" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1705,7 +1691,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1715,7 +1701,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1736,18 +1722,18 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E31" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="G32" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1845,18 +1831,18 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D45" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D46" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -1864,7 +1850,7 @@
         <v>167</v>
       </c>
       <c r="E47" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -1938,7 +1924,7 @@
         <v>197</v>
       </c>
       <c r="E57" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -1980,18 +1966,18 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D63" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E64" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -1999,7 +1985,7 @@
         <v>181</v>
       </c>
       <c r="G65" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2038,7 +2024,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E71" t="s">
         <v>205</v>
@@ -2046,10 +2032,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="G72" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -2091,7 +2077,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -2157,7 +2143,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D87" t="s">
         <v>221</v>
@@ -2165,7 +2151,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="E88" t="s">
         <v>222</v>
@@ -2197,7 +2183,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D92" t="s">
         <v>228</v>
@@ -2205,7 +2191,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="E93" t="s">
         <v>229</v>
@@ -2229,7 +2215,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D96" t="s">
         <v>233</v>
@@ -2237,23 +2223,23 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
+        <v>317</v>
+      </c>
+      <c r="E97" t="s">
         <v>234</v>
-      </c>
-      <c r="E97" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F98" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -2261,7 +2247,7 @@
         <v>144</v>
       </c>
       <c r="E100" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -2271,10 +2257,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>236</v>
+      </c>
+      <c r="E102" t="s">
         <v>237</v>
-      </c>
-      <c r="E102" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -2282,7 +2268,7 @@
         <v>3</v>
       </c>
       <c r="E103" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -2290,7 +2276,7 @@
         <v>9</v>
       </c>
       <c r="E104" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
@@ -2298,15 +2284,15 @@
         <v>181</v>
       </c>
       <c r="G105" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>242</v>
+        <v>318</v>
       </c>
       <c r="E106" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
@@ -2314,7 +2300,7 @@
         <v>183</v>
       </c>
       <c r="E107" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
@@ -2327,15 +2313,15 @@
         <v>181</v>
       </c>
       <c r="G109" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>245</v>
+        <v>319</v>
       </c>
       <c r="E110" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
@@ -2343,7 +2329,7 @@
         <v>183</v>
       </c>
       <c r="E111" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
@@ -2356,7 +2342,7 @@
         <v>181</v>
       </c>
       <c r="G113" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
@@ -2364,7 +2350,7 @@
         <v>183</v>
       </c>
       <c r="E114" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
@@ -2377,15 +2363,15 @@
         <v>10</v>
       </c>
       <c r="F116" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E117" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
@@ -2393,23 +2379,23 @@
         <v>11</v>
       </c>
       <c r="G118" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D119" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G120" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
@@ -2417,15 +2403,15 @@
         <v>12</v>
       </c>
       <c r="F121" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>255</v>
+        <v>320</v>
       </c>
       <c r="E122" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
@@ -2433,12 +2419,12 @@
         <v>188</v>
       </c>
       <c r="E123" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
@@ -2446,31 +2432,31 @@
         <v>11</v>
       </c>
       <c r="G125" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D126" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D127" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G128" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -2478,15 +2464,15 @@
         <v>12</v>
       </c>
       <c r="F129" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E130" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
@@ -2494,12 +2480,12 @@
         <v>188</v>
       </c>
       <c r="E131" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
@@ -2507,31 +2493,31 @@
         <v>11</v>
       </c>
       <c r="G133" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D134" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D135" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G136" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
@@ -2539,7 +2525,7 @@
         <v>12</v>
       </c>
       <c r="F137" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
@@ -2547,7 +2533,7 @@
         <v>3</v>
       </c>
       <c r="E138" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
@@ -2555,12 +2541,12 @@
         <v>188</v>
       </c>
       <c r="E139" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
@@ -2568,31 +2554,31 @@
         <v>11</v>
       </c>
       <c r="G141" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>310</v>
+        <v>321</v>
       </c>
       <c r="D142" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D143" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G144" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
@@ -2600,7 +2586,7 @@
         <v>191</v>
       </c>
       <c r="G145" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
@@ -2621,7 +2607,7 @@
         <v>13</v>
       </c>
       <c r="H148" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -2634,10 +2620,10 @@
   <dimension ref="A1:AD248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A149"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3086,7 +3072,7 @@
         <v/>
       </c>
       <c r="AB4" s="11" t="str">
-        <f t="shared" ref="AB3:AB66" si="29">W4&amp;X4&amp;Y4&amp;Z4&amp;AA4</f>
+        <f t="shared" ref="AB4:AB66" si="29">W4&amp;X4&amp;Y4&amp;Z4&amp;AA4</f>
         <v>0001101100000000</v>
       </c>
       <c r="AC4" s="10">
@@ -3447,7 +3433,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B8" s="9" t="str">
         <f t="shared" si="8"/>
@@ -3564,7 +3550,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B9" s="9" t="str">
         <f t="shared" si="8"/>
@@ -3915,7 +3901,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B12" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4032,7 +4018,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B13" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4617,7 +4603,7 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B18" s="9" t="str">
         <f t="shared" si="8"/>
@@ -4851,7 +4837,7 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B20" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5085,7 +5071,7 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B22" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5436,7 +5422,7 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B25" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5670,7 +5656,7 @@
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B27" s="9" t="str">
         <f t="shared" si="8"/>
@@ -5904,7 +5890,7 @@
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B29" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6255,7 +6241,7 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B32" s="9" t="str">
         <f t="shared" si="8"/>
@@ -6372,7 +6358,7 @@
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B33" s="9" t="str">
         <f t="shared" si="8"/>
@@ -7893,7 +7879,7 @@
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B46" s="9" t="str">
         <f t="shared" si="8"/>
@@ -8010,7 +7996,7 @@
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B47" s="9" t="str">
         <f t="shared" si="8"/>
@@ -9999,7 +9985,7 @@
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B64" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10116,7 +10102,7 @@
     </row>
     <row r="65" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B65" s="9" t="str">
         <f t="shared" si="8"/>
@@ -10935,7 +10921,7 @@
     </row>
     <row r="72" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A72" s="12" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B72" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11052,7 +11038,7 @@
     </row>
     <row r="73" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B73" s="9" t="str">
         <f t="shared" si="31"/>
@@ -11754,7 +11740,7 @@
     </row>
     <row r="79" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A79" s="12" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B79" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12807,7 +12793,7 @@
     </row>
     <row r="88" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A88" s="12" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B88" s="9" t="str">
         <f t="shared" si="31"/>
@@ -12924,7 +12910,7 @@
     </row>
     <row r="89" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B89" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13392,7 +13378,7 @@
     </row>
     <row r="93" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A93" s="12" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B93" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13509,7 +13495,7 @@
     </row>
     <row r="94" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A94" s="12" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B94" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13860,7 +13846,7 @@
     </row>
     <row r="97" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B97" s="9" t="str">
         <f t="shared" si="31"/>
@@ -13977,11 +13963,11 @@
     </row>
     <row r="98" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A98" s="12" t="s">
-        <v>234</v>
+        <v>317</v>
       </c>
       <c r="B98" s="9" t="str">
         <f t="shared" si="31"/>
-        <v>LDA</v>
+        <v>LDR</v>
       </c>
       <c r="C98" s="9">
         <f t="shared" si="32"/>
@@ -14025,7 +14011,7 @@
       </c>
       <c r="M98" s="22" t="str">
         <f>VLOOKUP($B98,'Conversion to binary Key'!$D:$I,2,0)</f>
-        <v>000011</v>
+        <v>000001</v>
       </c>
       <c r="N98" s="22" t="str">
         <f>VLOOKUP($B98,'Conversion to binary Key'!$D:$I,3,0)</f>
@@ -14045,7 +14031,7 @@
       </c>
       <c r="R98" s="17" t="str">
         <f t="shared" si="42"/>
-        <v>000011</v>
+        <v>000001</v>
       </c>
       <c r="S98" s="25" t="str">
         <f t="shared" si="43"/>
@@ -14065,7 +14051,7 @@
       </c>
       <c r="W98" s="15" t="str">
         <f t="shared" si="47"/>
-        <v>000011</v>
+        <v>000001</v>
       </c>
       <c r="X98" s="10" t="str">
         <f t="shared" si="48"/>
@@ -14085,7 +14071,7 @@
       </c>
       <c r="AB98" s="11" t="str">
         <f t="shared" si="52"/>
-        <v>0000111100011101</v>
+        <v>0000011100011101</v>
       </c>
       <c r="AC98" s="10">
         <f t="shared" si="30"/>
@@ -14094,7 +14080,7 @@
     </row>
     <row r="99" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A99" s="12" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B99" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14211,7 +14197,7 @@
     </row>
     <row r="100" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="B100" s="9" t="str">
         <f t="shared" si="31"/>
@@ -14562,7 +14548,7 @@
     </row>
     <row r="103" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B103" s="9" t="str">
         <f t="shared" si="31"/>
@@ -15030,11 +15016,11 @@
     </row>
     <row r="107" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A107" s="12" t="s">
-        <v>242</v>
+        <v>318</v>
       </c>
       <c r="B107" s="9" t="str">
         <f t="shared" si="31"/>
-        <v>LDR</v>
+        <v>STR</v>
       </c>
       <c r="C107" s="9">
         <f t="shared" si="32"/>
@@ -15078,7 +15064,7 @@
       </c>
       <c r="M107" s="22" t="str">
         <f>VLOOKUP($B107,'Conversion to binary Key'!$D:$I,2,0)</f>
-        <v>000001</v>
+        <v>000010</v>
       </c>
       <c r="N107" s="22" t="str">
         <f>VLOOKUP($B107,'Conversion to binary Key'!$D:$I,3,0)</f>
@@ -15098,7 +15084,7 @@
       </c>
       <c r="R107" s="17" t="str">
         <f t="shared" si="42"/>
-        <v>000001</v>
+        <v>000010</v>
       </c>
       <c r="S107" s="25" t="str">
         <f t="shared" si="43"/>
@@ -15118,7 +15104,7 @@
       </c>
       <c r="W107" s="15" t="str">
         <f t="shared" si="47"/>
-        <v>000001</v>
+        <v>000010</v>
       </c>
       <c r="X107" s="10" t="str">
         <f t="shared" si="48"/>
@@ -15138,7 +15124,7 @@
       </c>
       <c r="AB107" s="11" t="str">
         <f t="shared" si="52"/>
-        <v>0000010101011010</v>
+        <v>0000100101011010</v>
       </c>
       <c r="AC107" s="10">
         <f t="shared" si="30"/>
@@ -15498,11 +15484,11 @@
     </row>
     <row r="111" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A111" s="12" t="s">
-        <v>245</v>
+        <v>319</v>
       </c>
       <c r="B111" s="9" t="str">
         <f t="shared" si="31"/>
-        <v>LDR</v>
+        <v>STR</v>
       </c>
       <c r="C111" s="9">
         <f t="shared" si="32"/>
@@ -15546,7 +15532,7 @@
       </c>
       <c r="M111" s="22" t="str">
         <f>VLOOKUP($B111,'Conversion to binary Key'!$D:$I,2,0)</f>
-        <v>000001</v>
+        <v>000010</v>
       </c>
       <c r="N111" s="22" t="str">
         <f>VLOOKUP($B111,'Conversion to binary Key'!$D:$I,3,0)</f>
@@ -15566,7 +15552,7 @@
       </c>
       <c r="R111" s="17" t="str">
         <f t="shared" si="42"/>
-        <v>000001</v>
+        <v>000010</v>
       </c>
       <c r="S111" s="25" t="str">
         <f t="shared" si="43"/>
@@ -15586,7 +15572,7 @@
       </c>
       <c r="W111" s="15" t="str">
         <f t="shared" si="47"/>
-        <v>000001</v>
+        <v>000010</v>
       </c>
       <c r="X111" s="10" t="str">
         <f t="shared" si="48"/>
@@ -15606,7 +15592,7 @@
       </c>
       <c r="AB111" s="11" t="str">
         <f t="shared" si="52"/>
-        <v>0000010101011101</v>
+        <v>0000100101011101</v>
       </c>
       <c r="AC111" s="10">
         <f t="shared" si="30"/>
@@ -16317,7 +16303,7 @@
     </row>
     <row r="118" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A118" s="12" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B118" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16551,7 +16537,7 @@
     </row>
     <row r="120" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A120" s="12" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B120" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16668,7 +16654,7 @@
     </row>
     <row r="121" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A121" s="12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B121" s="9" t="str">
         <f t="shared" si="31"/>
@@ -16902,11 +16888,11 @@
     </row>
     <row r="123" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A123" s="12" t="s">
-        <v>255</v>
+        <v>320</v>
       </c>
       <c r="B123" s="9" t="str">
         <f t="shared" si="31"/>
-        <v>LDA</v>
+        <v>LDR</v>
       </c>
       <c r="C123" s="9">
         <f t="shared" si="32"/>
@@ -16950,7 +16936,7 @@
       </c>
       <c r="M123" s="22" t="str">
         <f>VLOOKUP($B123,'Conversion to binary Key'!$D:$I,2,0)</f>
-        <v>000011</v>
+        <v>000001</v>
       </c>
       <c r="N123" s="22" t="str">
         <f>VLOOKUP($B123,'Conversion to binary Key'!$D:$I,3,0)</f>
@@ -16970,7 +16956,7 @@
       </c>
       <c r="R123" s="17" t="str">
         <f t="shared" si="42"/>
-        <v>000011</v>
+        <v>000001</v>
       </c>
       <c r="S123" s="25" t="str">
         <f t="shared" si="43"/>
@@ -16990,7 +16976,7 @@
       </c>
       <c r="W123" s="15" t="str">
         <f t="shared" si="47"/>
-        <v>000011</v>
+        <v>000001</v>
       </c>
       <c r="X123" s="10" t="str">
         <f t="shared" si="48"/>
@@ -17010,7 +16996,7 @@
       </c>
       <c r="AB123" s="11" t="str">
         <f t="shared" si="52"/>
-        <v>0000110001011101</v>
+        <v>0000010001011101</v>
       </c>
       <c r="AC123" s="10">
         <f t="shared" si="30"/>
@@ -17136,7 +17122,7 @@
     </row>
     <row r="125" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A125" s="12" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B125" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17370,7 +17356,7 @@
     </row>
     <row r="127" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A127" s="12" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B127" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17487,7 +17473,7 @@
     </row>
     <row r="128" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A128" s="12" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B128" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17604,7 +17590,7 @@
     </row>
     <row r="129" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A129" s="12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B129" s="9" t="str">
         <f t="shared" si="31"/>
@@ -17838,7 +17824,7 @@
     </row>
     <row r="131" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A131" s="12" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B131" s="9" t="str">
         <f t="shared" ref="B131:B146" si="54">LEFT(A131,3)</f>
@@ -18072,7 +18058,7 @@
     </row>
     <row r="133" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A133" s="12" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B133" s="9" t="str">
         <f t="shared" si="54"/>
@@ -18306,7 +18292,7 @@
     </row>
     <row r="135" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A135" s="12" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B135" s="9" t="str">
         <f t="shared" si="54"/>
@@ -18423,7 +18409,7 @@
     </row>
     <row r="136" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A136" s="12" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B136" s="9" t="str">
         <f t="shared" si="54"/>
@@ -18540,7 +18526,7 @@
     </row>
     <row r="137" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A137" s="12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B137" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19008,7 +18994,7 @@
     </row>
     <row r="141" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A141" s="12" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B141" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19242,7 +19228,7 @@
     </row>
     <row r="143" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A143" s="12" t="s">
-        <v>310</v>
+        <v>321</v>
       </c>
       <c r="B143" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19274,7 +19260,7 @@
       </c>
       <c r="I143" s="9" t="str">
         <f t="shared" si="61"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J143" s="9" t="str">
         <f t="shared" si="62"/>
@@ -19314,7 +19300,7 @@
       </c>
       <c r="S143" s="25" t="str">
         <f t="shared" si="66"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T143" s="25" t="str">
         <f t="shared" si="67"/>
@@ -19334,7 +19320,7 @@
       </c>
       <c r="X143" s="10" t="str">
         <f t="shared" si="71"/>
-        <v>01</v>
+        <v>10</v>
       </c>
       <c r="Y143" s="10" t="str">
         <f t="shared" si="72"/>
@@ -19350,7 +19336,7 @@
       </c>
       <c r="AB143" s="11" t="str">
         <f t="shared" si="75"/>
-        <v>0010000111011001</v>
+        <v>0010001011011001</v>
       </c>
       <c r="AC143" s="10">
         <f t="shared" si="53"/>
@@ -19359,7 +19345,7 @@
     </row>
     <row r="144" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A144" s="12" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B144" s="9" t="str">
         <f t="shared" si="54"/>
@@ -19476,7 +19462,7 @@
     </row>
     <row r="145" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A145" s="12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B145" s="9" t="str">
         <f t="shared" si="54"/>
@@ -20656,7 +20642,7 @@
   </sheetData>
   <autoFilter ref="A1:AC146"/>
   <conditionalFormatting sqref="AC2:AC149">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>